<commit_message>
languages in xslx in english
</commit_message>
<xml_diff>
--- a/01_input/swiss_teams_lamguage.xlsx
+++ b/01_input/swiss_teams_lamguage.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/nicowyss/Documents/Git/social_analysis_football_transfer/01_input/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EC41660E-27DB-4049-A21D-9522B6E1EC32}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{523D3387-C37B-9647-B05B-69BD5FD22230}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-20" yWindow="520" windowWidth="33600" windowHeight="20500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -16,14 +16,14 @@
     <sheet name="swiss_teams_lamguage" sheetId="1" r:id="rId1"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">swiss_teams_lamguage!$A$1:$C$162</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">swiss_teams_lamguage!$A$1:$D$162</definedName>
   </definedNames>
   <calcPr calcId="0"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="486" uniqueCount="168">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="648" uniqueCount="171">
   <si>
     <t>FC Prilly</t>
   </si>
@@ -520,13 +520,22 @@
     <t>Sprache</t>
   </si>
   <si>
-    <t>Deutsch</t>
-  </si>
-  <si>
-    <t>Italienisch</t>
-  </si>
-  <si>
-    <t>Französisch</t>
+    <t>German</t>
+  </si>
+  <si>
+    <t>Italian</t>
+  </si>
+  <si>
+    <t>French</t>
+  </si>
+  <si>
+    <t>Language Familiy</t>
+  </si>
+  <si>
+    <t>Romance</t>
+  </si>
+  <si>
+    <t>Germanic</t>
   </si>
 </sst>
 </file>
@@ -1367,18 +1376,19 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:C162"/>
+  <dimension ref="A1:D162"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A115" workbookViewId="0">
-      <selection activeCell="D159" sqref="D159"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="J23" sqref="J23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="33.5" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="15.5" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>162</v>
       </c>
@@ -1388,8 +1398,11 @@
       <c r="C1" t="s">
         <v>164</v>
       </c>
-    </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D1" t="s">
+        <v>168</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>114</v>
       </c>
@@ -1399,8 +1412,11 @@
       <c r="C2" t="s">
         <v>166</v>
       </c>
-    </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D2" t="s">
+        <v>169</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>82</v>
       </c>
@@ -1410,8 +1426,11 @@
       <c r="C3" t="s">
         <v>165</v>
       </c>
-    </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D3" t="s">
+        <v>170</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
         <v>64</v>
       </c>
@@ -1421,8 +1440,11 @@
       <c r="C4" t="s">
         <v>165</v>
       </c>
-    </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D4" t="s">
+        <v>170</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
         <v>2</v>
       </c>
@@ -1432,8 +1454,11 @@
       <c r="C5" t="s">
         <v>165</v>
       </c>
-    </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D5" t="s">
+        <v>170</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
         <v>16</v>
       </c>
@@ -1443,8 +1468,11 @@
       <c r="C6" t="s">
         <v>166</v>
       </c>
-    </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D6" t="s">
+        <v>169</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
         <v>41</v>
       </c>
@@ -1454,8 +1482,11 @@
       <c r="C7" t="s">
         <v>166</v>
       </c>
-    </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D7" t="s">
+        <v>169</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
         <v>43</v>
       </c>
@@ -1465,8 +1496,11 @@
       <c r="C8" t="s">
         <v>166</v>
       </c>
-    </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D8" t="s">
+        <v>169</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
         <v>38</v>
       </c>
@@ -1476,8 +1510,11 @@
       <c r="C9" t="s">
         <v>166</v>
       </c>
-    </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D9" t="s">
+        <v>169</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
         <v>95</v>
       </c>
@@ -1487,8 +1524,11 @@
       <c r="C10" t="s">
         <v>166</v>
       </c>
-    </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D10" t="s">
+        <v>169</v>
+      </c>
+    </row>
+    <row r="11" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
         <v>124</v>
       </c>
@@ -1498,8 +1538,11 @@
       <c r="C11" t="s">
         <v>166</v>
       </c>
-    </row>
-    <row r="12" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D11" t="s">
+        <v>169</v>
+      </c>
+    </row>
+    <row r="12" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
         <v>34</v>
       </c>
@@ -1509,8 +1552,11 @@
       <c r="C12" t="s">
         <v>166</v>
       </c>
-    </row>
-    <row r="13" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D12" t="s">
+        <v>169</v>
+      </c>
+    </row>
+    <row r="13" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
         <v>35</v>
       </c>
@@ -1520,8 +1566,11 @@
       <c r="C13" t="s">
         <v>166</v>
       </c>
-    </row>
-    <row r="14" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D13" t="s">
+        <v>169</v>
+      </c>
+    </row>
+    <row r="14" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A14" t="s">
         <v>53</v>
       </c>
@@ -1531,8 +1580,11 @@
       <c r="C14" t="s">
         <v>166</v>
       </c>
-    </row>
-    <row r="15" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D14" t="s">
+        <v>169</v>
+      </c>
+    </row>
+    <row r="15" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A15" t="s">
         <v>161</v>
       </c>
@@ -1542,8 +1594,11 @@
       <c r="C15" t="s">
         <v>166</v>
       </c>
-    </row>
-    <row r="16" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D15" t="s">
+        <v>169</v>
+      </c>
+    </row>
+    <row r="16" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A16" t="s">
         <v>123</v>
       </c>
@@ -1553,8 +1608,11 @@
       <c r="C16" t="s">
         <v>166</v>
       </c>
-    </row>
-    <row r="17" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D16" t="s">
+        <v>169</v>
+      </c>
+    </row>
+    <row r="17" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A17" t="s">
         <v>28</v>
       </c>
@@ -1564,8 +1622,11 @@
       <c r="C17" t="s">
         <v>166</v>
       </c>
-    </row>
-    <row r="18" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D17" t="s">
+        <v>169</v>
+      </c>
+    </row>
+    <row r="18" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A18" t="s">
         <v>51</v>
       </c>
@@ -1575,8 +1636,11 @@
       <c r="C18" t="s">
         <v>165</v>
       </c>
-    </row>
-    <row r="19" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D18" t="s">
+        <v>170</v>
+      </c>
+    </row>
+    <row r="19" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A19" t="s">
         <v>86</v>
       </c>
@@ -1586,8 +1650,11 @@
       <c r="C19" t="s">
         <v>165</v>
       </c>
-    </row>
-    <row r="20" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D19" t="s">
+        <v>170</v>
+      </c>
+    </row>
+    <row r="20" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A20" t="s">
         <v>7</v>
       </c>
@@ -1597,8 +1664,11 @@
       <c r="C20" t="s">
         <v>165</v>
       </c>
-    </row>
-    <row r="21" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D20" t="s">
+        <v>170</v>
+      </c>
+    </row>
+    <row r="21" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A21" t="s">
         <v>40</v>
       </c>
@@ -1608,8 +1678,11 @@
       <c r="C21" t="s">
         <v>165</v>
       </c>
-    </row>
-    <row r="22" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D21" t="s">
+        <v>170</v>
+      </c>
+    </row>
+    <row r="22" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A22" t="s">
         <v>48</v>
       </c>
@@ -1619,8 +1692,11 @@
       <c r="C22" t="s">
         <v>167</v>
       </c>
-    </row>
-    <row r="23" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D22" t="s">
+        <v>169</v>
+      </c>
+    </row>
+    <row r="23" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A23" t="s">
         <v>13</v>
       </c>
@@ -1630,8 +1706,11 @@
       <c r="C23" t="s">
         <v>165</v>
       </c>
-    </row>
-    <row r="24" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D23" t="s">
+        <v>170</v>
+      </c>
+    </row>
+    <row r="24" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A24" t="s">
         <v>109</v>
       </c>
@@ -1641,8 +1720,11 @@
       <c r="C24" t="s">
         <v>167</v>
       </c>
-    </row>
-    <row r="25" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D24" t="s">
+        <v>169</v>
+      </c>
+    </row>
+    <row r="25" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A25" t="s">
         <v>151</v>
       </c>
@@ -1652,8 +1734,11 @@
       <c r="C25" t="s">
         <v>165</v>
       </c>
-    </row>
-    <row r="26" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D25" t="s">
+        <v>170</v>
+      </c>
+    </row>
+    <row r="26" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A26" t="s">
         <v>39</v>
       </c>
@@ -1663,8 +1748,11 @@
       <c r="C26" t="s">
         <v>167</v>
       </c>
-    </row>
-    <row r="27" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D26" t="s">
+        <v>169</v>
+      </c>
+    </row>
+    <row r="27" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A27" t="s">
         <v>3</v>
       </c>
@@ -1674,8 +1762,11 @@
       <c r="C27" t="s">
         <v>165</v>
       </c>
-    </row>
-    <row r="28" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D27" t="s">
+        <v>170</v>
+      </c>
+    </row>
+    <row r="28" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A28" t="s">
         <v>33</v>
       </c>
@@ -1685,8 +1776,11 @@
       <c r="C28" t="s">
         <v>165</v>
       </c>
-    </row>
-    <row r="29" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D28" t="s">
+        <v>170</v>
+      </c>
+    </row>
+    <row r="29" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A29" t="s">
         <v>98</v>
       </c>
@@ -1696,8 +1790,11 @@
       <c r="C29" t="s">
         <v>165</v>
       </c>
-    </row>
-    <row r="30" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D29" t="s">
+        <v>170</v>
+      </c>
+    </row>
+    <row r="30" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A30" t="s">
         <v>130</v>
       </c>
@@ -1707,8 +1804,11 @@
       <c r="C30" t="s">
         <v>167</v>
       </c>
-    </row>
-    <row r="31" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D30" t="s">
+        <v>169</v>
+      </c>
+    </row>
+    <row r="31" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A31" t="s">
         <v>105</v>
       </c>
@@ -1718,8 +1818,11 @@
       <c r="C31" t="s">
         <v>167</v>
       </c>
-    </row>
-    <row r="32" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D31" t="s">
+        <v>169</v>
+      </c>
+    </row>
+    <row r="32" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A32" t="s">
         <v>102</v>
       </c>
@@ -1729,8 +1832,11 @@
       <c r="C32" t="s">
         <v>166</v>
       </c>
-    </row>
-    <row r="33" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D32" t="s">
+        <v>169</v>
+      </c>
+    </row>
+    <row r="33" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A33" t="s">
         <v>111</v>
       </c>
@@ -1740,8 +1846,11 @@
       <c r="C33" t="s">
         <v>165</v>
       </c>
-    </row>
-    <row r="34" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D33" t="s">
+        <v>170</v>
+      </c>
+    </row>
+    <row r="34" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A34" t="s">
         <v>94</v>
       </c>
@@ -1751,8 +1860,11 @@
       <c r="C34" t="s">
         <v>165</v>
       </c>
-    </row>
-    <row r="35" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D34" t="s">
+        <v>170</v>
+      </c>
+    </row>
+    <row r="35" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A35" t="s">
         <v>30</v>
       </c>
@@ -1762,8 +1874,11 @@
       <c r="C35" t="s">
         <v>165</v>
       </c>
-    </row>
-    <row r="36" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D35" t="s">
+        <v>170</v>
+      </c>
+    </row>
+    <row r="36" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A36" t="s">
         <v>22</v>
       </c>
@@ -1773,8 +1888,11 @@
       <c r="C36" t="s">
         <v>165</v>
       </c>
-    </row>
-    <row r="37" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D36" t="s">
+        <v>170</v>
+      </c>
+    </row>
+    <row r="37" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A37" t="s">
         <v>59</v>
       </c>
@@ -1784,8 +1902,11 @@
       <c r="C37" t="s">
         <v>165</v>
       </c>
-    </row>
-    <row r="38" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D37" t="s">
+        <v>170</v>
+      </c>
+    </row>
+    <row r="38" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A38" t="s">
         <v>132</v>
       </c>
@@ -1795,8 +1916,11 @@
       <c r="C38" t="s">
         <v>165</v>
       </c>
-    </row>
-    <row r="39" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D38" t="s">
+        <v>170</v>
+      </c>
+    </row>
+    <row r="39" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A39" t="s">
         <v>133</v>
       </c>
@@ -1806,8 +1930,11 @@
       <c r="C39" t="s">
         <v>167</v>
       </c>
-    </row>
-    <row r="40" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D39" t="s">
+        <v>169</v>
+      </c>
+    </row>
+    <row r="40" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A40" t="s">
         <v>91</v>
       </c>
@@ -1817,8 +1944,11 @@
       <c r="C40" t="s">
         <v>167</v>
       </c>
-    </row>
-    <row r="41" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D40" t="s">
+        <v>169</v>
+      </c>
+    </row>
+    <row r="41" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A41" t="s">
         <v>138</v>
       </c>
@@ -1828,8 +1958,11 @@
       <c r="C41" t="s">
         <v>167</v>
       </c>
-    </row>
-    <row r="42" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D41" t="s">
+        <v>169</v>
+      </c>
+    </row>
+    <row r="42" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A42" t="s">
         <v>115</v>
       </c>
@@ -1839,8 +1972,11 @@
       <c r="C42" t="s">
         <v>165</v>
       </c>
-    </row>
-    <row r="43" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D42" t="s">
+        <v>170</v>
+      </c>
+    </row>
+    <row r="43" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A43" t="s">
         <v>145</v>
       </c>
@@ -1850,8 +1986,11 @@
       <c r="C43" t="s">
         <v>165</v>
       </c>
-    </row>
-    <row r="44" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D43" t="s">
+        <v>170</v>
+      </c>
+    </row>
+    <row r="44" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A44" t="s">
         <v>19</v>
       </c>
@@ -1861,8 +2000,11 @@
       <c r="C44" t="s">
         <v>165</v>
       </c>
-    </row>
-    <row r="45" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D44" t="s">
+        <v>170</v>
+      </c>
+    </row>
+    <row r="45" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A45" t="s">
         <v>4</v>
       </c>
@@ -1872,8 +2014,11 @@
       <c r="C45" t="s">
         <v>166</v>
       </c>
-    </row>
-    <row r="46" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D45" t="s">
+        <v>169</v>
+      </c>
+    </row>
+    <row r="46" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A46" t="s">
         <v>58</v>
       </c>
@@ -1883,8 +2028,11 @@
       <c r="C46" t="s">
         <v>166</v>
       </c>
-    </row>
-    <row r="47" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D46" t="s">
+        <v>169</v>
+      </c>
+    </row>
+    <row r="47" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A47" t="s">
         <v>75</v>
       </c>
@@ -1894,8 +2042,11 @@
       <c r="C47" t="s">
         <v>167</v>
       </c>
-    </row>
-    <row r="48" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D47" t="s">
+        <v>169</v>
+      </c>
+    </row>
+    <row r="48" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A48" t="s">
         <v>129</v>
       </c>
@@ -1905,8 +2056,11 @@
       <c r="C48" t="s">
         <v>167</v>
       </c>
-    </row>
-    <row r="49" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D48" t="s">
+        <v>169</v>
+      </c>
+    </row>
+    <row r="49" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A49" t="s">
         <v>125</v>
       </c>
@@ -1916,8 +2070,11 @@
       <c r="C49" t="s">
         <v>165</v>
       </c>
-    </row>
-    <row r="50" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D49" t="s">
+        <v>170</v>
+      </c>
+    </row>
+    <row r="50" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A50" t="s">
         <v>107</v>
       </c>
@@ -1927,8 +2084,11 @@
       <c r="C50" t="s">
         <v>165</v>
       </c>
-    </row>
-    <row r="51" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D50" t="s">
+        <v>170</v>
+      </c>
+    </row>
+    <row r="51" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A51" t="s">
         <v>104</v>
       </c>
@@ -1938,8 +2098,11 @@
       <c r="C51" t="s">
         <v>167</v>
       </c>
-    </row>
-    <row r="52" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D51" t="s">
+        <v>169</v>
+      </c>
+    </row>
+    <row r="52" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A52" t="s">
         <v>147</v>
       </c>
@@ -1949,8 +2112,11 @@
       <c r="C52" t="s">
         <v>165</v>
       </c>
-    </row>
-    <row r="53" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D52" t="s">
+        <v>170</v>
+      </c>
+    </row>
+    <row r="53" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A53" t="s">
         <v>56</v>
       </c>
@@ -1960,8 +2126,11 @@
       <c r="C53" t="s">
         <v>165</v>
       </c>
-    </row>
-    <row r="54" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D53" t="s">
+        <v>170</v>
+      </c>
+    </row>
+    <row r="54" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A54" t="s">
         <v>154</v>
       </c>
@@ -1971,8 +2140,11 @@
       <c r="C54" t="s">
         <v>167</v>
       </c>
-    </row>
-    <row r="55" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D54" t="s">
+        <v>169</v>
+      </c>
+    </row>
+    <row r="55" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A55" t="s">
         <v>61</v>
       </c>
@@ -1982,8 +2154,11 @@
       <c r="C55" t="s">
         <v>165</v>
       </c>
-    </row>
-    <row r="56" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D55" t="s">
+        <v>170</v>
+      </c>
+    </row>
+    <row r="56" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A56" t="s">
         <v>70</v>
       </c>
@@ -1993,8 +2168,11 @@
       <c r="C56" t="s">
         <v>167</v>
       </c>
-    </row>
-    <row r="57" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D56" t="s">
+        <v>169</v>
+      </c>
+    </row>
+    <row r="57" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A57" t="s">
         <v>76</v>
       </c>
@@ -2004,8 +2182,11 @@
       <c r="C57" t="s">
         <v>166</v>
       </c>
-    </row>
-    <row r="58" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D57" t="s">
+        <v>169</v>
+      </c>
+    </row>
+    <row r="58" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A58" t="s">
         <v>26</v>
       </c>
@@ -2015,8 +2196,11 @@
       <c r="C58" t="s">
         <v>165</v>
       </c>
-    </row>
-    <row r="59" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D58" t="s">
+        <v>170</v>
+      </c>
+    </row>
+    <row r="59" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A59" t="s">
         <v>101</v>
       </c>
@@ -2026,8 +2210,11 @@
       <c r="C59" t="s">
         <v>165</v>
       </c>
-    </row>
-    <row r="60" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D59" t="s">
+        <v>170</v>
+      </c>
+    </row>
+    <row r="60" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A60" t="s">
         <v>122</v>
       </c>
@@ -2037,8 +2224,11 @@
       <c r="C60" t="s">
         <v>165</v>
       </c>
-    </row>
-    <row r="61" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D60" t="s">
+        <v>170</v>
+      </c>
+    </row>
+    <row r="61" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A61" t="s">
         <v>60</v>
       </c>
@@ -2048,8 +2238,11 @@
       <c r="C61" t="s">
         <v>165</v>
       </c>
-    </row>
-    <row r="62" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D61" t="s">
+        <v>170</v>
+      </c>
+    </row>
+    <row r="62" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A62" t="s">
         <v>65</v>
       </c>
@@ -2059,8 +2252,11 @@
       <c r="C62" t="s">
         <v>167</v>
       </c>
-    </row>
-    <row r="63" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D62" t="s">
+        <v>169</v>
+      </c>
+    </row>
+    <row r="63" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A63" t="s">
         <v>112</v>
       </c>
@@ -2070,8 +2266,11 @@
       <c r="C63" t="s">
         <v>165</v>
       </c>
-    </row>
-    <row r="64" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D63" t="s">
+        <v>170</v>
+      </c>
+    </row>
+    <row r="64" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A64" t="s">
         <v>20</v>
       </c>
@@ -2081,8 +2280,11 @@
       <c r="C64" t="s">
         <v>165</v>
       </c>
-    </row>
-    <row r="65" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D64" t="s">
+        <v>170</v>
+      </c>
+    </row>
+    <row r="65" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A65" t="s">
         <v>57</v>
       </c>
@@ -2092,8 +2294,11 @@
       <c r="C65" t="s">
         <v>166</v>
       </c>
-    </row>
-    <row r="66" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D65" t="s">
+        <v>169</v>
+      </c>
+    </row>
+    <row r="66" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A66" t="s">
         <v>42</v>
       </c>
@@ -2103,8 +2308,11 @@
       <c r="C66" t="s">
         <v>166</v>
       </c>
-    </row>
-    <row r="67" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D66" t="s">
+        <v>169</v>
+      </c>
+    </row>
+    <row r="67" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A67" t="s">
         <v>80</v>
       </c>
@@ -2114,8 +2322,11 @@
       <c r="C67" t="s">
         <v>166</v>
       </c>
-    </row>
-    <row r="68" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D67" t="s">
+        <v>169</v>
+      </c>
+    </row>
+    <row r="68" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A68" t="s">
         <v>96</v>
       </c>
@@ -2125,8 +2336,11 @@
       <c r="C68" t="s">
         <v>165</v>
       </c>
-    </row>
-    <row r="69" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D68" t="s">
+        <v>170</v>
+      </c>
+    </row>
+    <row r="69" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A69" t="s">
         <v>83</v>
       </c>
@@ -2136,8 +2350,11 @@
       <c r="C69" t="s">
         <v>166</v>
       </c>
-    </row>
-    <row r="70" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D69" t="s">
+        <v>169</v>
+      </c>
+    </row>
+    <row r="70" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A70" t="s">
         <v>92</v>
       </c>
@@ -2147,8 +2364,11 @@
       <c r="C70" t="s">
         <v>166</v>
       </c>
-    </row>
-    <row r="71" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D70" t="s">
+        <v>169</v>
+      </c>
+    </row>
+    <row r="71" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A71" t="s">
         <v>23</v>
       </c>
@@ -2158,8 +2378,11 @@
       <c r="C71" t="s">
         <v>167</v>
       </c>
-    </row>
-    <row r="72" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D71" t="s">
+        <v>169</v>
+      </c>
+    </row>
+    <row r="72" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A72" t="s">
         <v>158</v>
       </c>
@@ -2169,8 +2392,11 @@
       <c r="C72" t="s">
         <v>165</v>
       </c>
-    </row>
-    <row r="73" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D72" t="s">
+        <v>170</v>
+      </c>
+    </row>
+    <row r="73" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A73" t="s">
         <v>144</v>
       </c>
@@ -2180,8 +2406,11 @@
       <c r="C73" t="s">
         <v>165</v>
       </c>
-    </row>
-    <row r="74" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D73" t="s">
+        <v>170</v>
+      </c>
+    </row>
+    <row r="74" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A74" t="s">
         <v>5</v>
       </c>
@@ -2191,8 +2420,11 @@
       <c r="C74" t="s">
         <v>165</v>
       </c>
-    </row>
-    <row r="75" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D74" t="s">
+        <v>170</v>
+      </c>
+    </row>
+    <row r="75" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A75" t="s">
         <v>160</v>
       </c>
@@ -2202,8 +2434,11 @@
       <c r="C75" t="s">
         <v>166</v>
       </c>
-    </row>
-    <row r="76" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D75" t="s">
+        <v>169</v>
+      </c>
+    </row>
+    <row r="76" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A76" t="s">
         <v>8</v>
       </c>
@@ -2213,8 +2448,11 @@
       <c r="C76" t="s">
         <v>167</v>
       </c>
-    </row>
-    <row r="77" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D76" t="s">
+        <v>169</v>
+      </c>
+    </row>
+    <row r="77" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A77" t="s">
         <v>49</v>
       </c>
@@ -2224,8 +2462,11 @@
       <c r="C77" t="s">
         <v>166</v>
       </c>
-    </row>
-    <row r="78" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D77" t="s">
+        <v>169</v>
+      </c>
+    </row>
+    <row r="78" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A78" t="s">
         <v>0</v>
       </c>
@@ -2235,8 +2476,11 @@
       <c r="C78" t="s">
         <v>167</v>
       </c>
-    </row>
-    <row r="79" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D78" t="s">
+        <v>169</v>
+      </c>
+    </row>
+    <row r="79" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A79" t="s">
         <v>135</v>
       </c>
@@ -2246,8 +2490,11 @@
       <c r="C79" t="s">
         <v>165</v>
       </c>
-    </row>
-    <row r="80" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D79" t="s">
+        <v>170</v>
+      </c>
+    </row>
+    <row r="80" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A80" t="s">
         <v>47</v>
       </c>
@@ -2257,8 +2504,11 @@
       <c r="C80" t="s">
         <v>165</v>
       </c>
-    </row>
-    <row r="81" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D80" t="s">
+        <v>170</v>
+      </c>
+    </row>
+    <row r="81" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A81" t="s">
         <v>116</v>
       </c>
@@ -2268,8 +2518,11 @@
       <c r="C81" t="s">
         <v>167</v>
       </c>
-    </row>
-    <row r="82" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D81" t="s">
+        <v>169</v>
+      </c>
+    </row>
+    <row r="82" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A82" t="s">
         <v>100</v>
       </c>
@@ -2279,8 +2532,11 @@
       <c r="C82" t="s">
         <v>167</v>
       </c>
-    </row>
-    <row r="83" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D82" t="s">
+        <v>169</v>
+      </c>
+    </row>
+    <row r="83" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A83" t="s">
         <v>113</v>
       </c>
@@ -2290,8 +2546,11 @@
       <c r="C83" t="s">
         <v>167</v>
       </c>
-    </row>
-    <row r="84" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D83" t="s">
+        <v>169</v>
+      </c>
+    </row>
+    <row r="84" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A84" t="s">
         <v>89</v>
       </c>
@@ -2301,8 +2560,11 @@
       <c r="C84" t="s">
         <v>167</v>
       </c>
-    </row>
-    <row r="85" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D84" t="s">
+        <v>169</v>
+      </c>
+    </row>
+    <row r="85" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A85" t="s">
         <v>55</v>
       </c>
@@ -2312,8 +2574,11 @@
       <c r="C85" t="s">
         <v>167</v>
       </c>
-    </row>
-    <row r="86" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D85" t="s">
+        <v>169</v>
+      </c>
+    </row>
+    <row r="86" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A86" t="s">
         <v>84</v>
       </c>
@@ -2323,8 +2588,11 @@
       <c r="C86" t="s">
         <v>165</v>
       </c>
-    </row>
-    <row r="87" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D86" t="s">
+        <v>170</v>
+      </c>
+    </row>
+    <row r="87" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A87" t="s">
         <v>131</v>
       </c>
@@ -2334,8 +2602,11 @@
       <c r="C87" t="s">
         <v>165</v>
       </c>
-    </row>
-    <row r="88" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D87" t="s">
+        <v>170</v>
+      </c>
+    </row>
+    <row r="88" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A88" t="s">
         <v>77</v>
       </c>
@@ -2345,8 +2616,11 @@
       <c r="C88" t="s">
         <v>165</v>
       </c>
-    </row>
-    <row r="89" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D88" t="s">
+        <v>170</v>
+      </c>
+    </row>
+    <row r="89" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A89" t="s">
         <v>37</v>
       </c>
@@ -2356,8 +2630,11 @@
       <c r="C89" t="s">
         <v>165</v>
       </c>
-    </row>
-    <row r="90" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D89" t="s">
+        <v>170</v>
+      </c>
+    </row>
+    <row r="90" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A90" t="s">
         <v>108</v>
       </c>
@@ -2367,8 +2644,11 @@
       <c r="C90" t="s">
         <v>165</v>
       </c>
-    </row>
-    <row r="91" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D90" t="s">
+        <v>170</v>
+      </c>
+    </row>
+    <row r="91" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A91" t="s">
         <v>85</v>
       </c>
@@ -2378,8 +2658,11 @@
       <c r="C91" t="s">
         <v>165</v>
       </c>
-    </row>
-    <row r="92" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D91" t="s">
+        <v>170</v>
+      </c>
+    </row>
+    <row r="92" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A92" t="s">
         <v>74</v>
       </c>
@@ -2389,8 +2672,11 @@
       <c r="C92" t="s">
         <v>165</v>
       </c>
-    </row>
-    <row r="93" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D92" t="s">
+        <v>170</v>
+      </c>
+    </row>
+    <row r="93" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A93" t="s">
         <v>73</v>
       </c>
@@ -2400,8 +2686,11 @@
       <c r="C93" t="s">
         <v>165</v>
       </c>
-    </row>
-    <row r="94" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D93" t="s">
+        <v>170</v>
+      </c>
+    </row>
+    <row r="94" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A94" t="s">
         <v>69</v>
       </c>
@@ -2411,8 +2700,11 @@
       <c r="C94" t="s">
         <v>165</v>
       </c>
-    </row>
-    <row r="95" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D94" t="s">
+        <v>170</v>
+      </c>
+    </row>
+    <row r="95" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A95" t="s">
         <v>50</v>
       </c>
@@ -2422,8 +2714,11 @@
       <c r="C95" t="s">
         <v>165</v>
       </c>
-    </row>
-    <row r="96" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D95" t="s">
+        <v>170</v>
+      </c>
+    </row>
+    <row r="96" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A96" t="s">
         <v>54</v>
       </c>
@@ -2433,8 +2728,11 @@
       <c r="C96" t="s">
         <v>165</v>
       </c>
-    </row>
-    <row r="97" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D96" t="s">
+        <v>170</v>
+      </c>
+    </row>
+    <row r="97" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A97" t="s">
         <v>36</v>
       </c>
@@ -2444,8 +2742,11 @@
       <c r="C97" t="s">
         <v>165</v>
       </c>
-    </row>
-    <row r="98" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D97" t="s">
+        <v>170</v>
+      </c>
+    </row>
+    <row r="98" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A98" t="s">
         <v>156</v>
       </c>
@@ -2455,8 +2756,11 @@
       <c r="C98" t="s">
         <v>165</v>
       </c>
-    </row>
-    <row r="99" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D98" t="s">
+        <v>170</v>
+      </c>
+    </row>
+    <row r="99" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A99" t="s">
         <v>32</v>
       </c>
@@ -2466,8 +2770,11 @@
       <c r="C99" t="s">
         <v>165</v>
       </c>
-    </row>
-    <row r="100" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D99" t="s">
+        <v>170</v>
+      </c>
+    </row>
+    <row r="100" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A100" t="s">
         <v>68</v>
       </c>
@@ -2477,8 +2784,11 @@
       <c r="C100" t="s">
         <v>165</v>
       </c>
-    </row>
-    <row r="101" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D100" t="s">
+        <v>170</v>
+      </c>
+    </row>
+    <row r="101" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A101" t="s">
         <v>25</v>
       </c>
@@ -2488,8 +2798,11 @@
       <c r="C101" t="s">
         <v>165</v>
       </c>
-    </row>
-    <row r="102" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D101" t="s">
+        <v>170</v>
+      </c>
+    </row>
+    <row r="102" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A102" t="s">
         <v>103</v>
       </c>
@@ -2499,8 +2812,11 @@
       <c r="C102" t="s">
         <v>165</v>
       </c>
-    </row>
-    <row r="103" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D102" t="s">
+        <v>170</v>
+      </c>
+    </row>
+    <row r="103" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A103" t="s">
         <v>119</v>
       </c>
@@ -2510,8 +2826,11 @@
       <c r="C103" t="s">
         <v>165</v>
       </c>
-    </row>
-    <row r="104" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D103" t="s">
+        <v>170</v>
+      </c>
+    </row>
+    <row r="104" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A104" t="s">
         <v>87</v>
       </c>
@@ -2521,8 +2840,11 @@
       <c r="C104" t="s">
         <v>165</v>
       </c>
-    </row>
-    <row r="105" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D104" t="s">
+        <v>170</v>
+      </c>
+    </row>
+    <row r="105" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A105" t="s">
         <v>121</v>
       </c>
@@ -2532,8 +2854,11 @@
       <c r="C105" t="s">
         <v>165</v>
       </c>
-    </row>
-    <row r="106" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D105" t="s">
+        <v>170</v>
+      </c>
+    </row>
+    <row r="106" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A106" t="s">
         <v>10</v>
       </c>
@@ -2543,8 +2868,11 @@
       <c r="C106" t="s">
         <v>166</v>
       </c>
-    </row>
-    <row r="107" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D106" t="s">
+        <v>169</v>
+      </c>
+    </row>
+    <row r="107" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A107" t="s">
         <v>106</v>
       </c>
@@ -2554,8 +2882,11 @@
       <c r="C107" t="s">
         <v>165</v>
       </c>
-    </row>
-    <row r="108" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D107" t="s">
+        <v>170</v>
+      </c>
+    </row>
+    <row r="108" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A108" t="s">
         <v>21</v>
       </c>
@@ -2565,8 +2896,11 @@
       <c r="C108" t="s">
         <v>165</v>
       </c>
-    </row>
-    <row r="109" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D108" t="s">
+        <v>170</v>
+      </c>
+    </row>
+    <row r="109" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A109" t="s">
         <v>6</v>
       </c>
@@ -2576,8 +2910,11 @@
       <c r="C109" t="s">
         <v>165</v>
       </c>
-    </row>
-    <row r="110" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D109" t="s">
+        <v>170</v>
+      </c>
+    </row>
+    <row r="110" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A110" t="s">
         <v>67</v>
       </c>
@@ -2587,8 +2924,11 @@
       <c r="C110" t="s">
         <v>165</v>
       </c>
-    </row>
-    <row r="111" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D110" t="s">
+        <v>170</v>
+      </c>
+    </row>
+    <row r="111" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A111" t="s">
         <v>81</v>
       </c>
@@ -2598,8 +2938,11 @@
       <c r="C111" t="s">
         <v>167</v>
       </c>
-    </row>
-    <row r="112" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D111" t="s">
+        <v>169</v>
+      </c>
+    </row>
+    <row r="112" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A112" t="s">
         <v>52</v>
       </c>
@@ -2609,8 +2952,11 @@
       <c r="C112" t="s">
         <v>167</v>
       </c>
-    </row>
-    <row r="113" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D112" t="s">
+        <v>169</v>
+      </c>
+    </row>
+    <row r="113" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A113" t="s">
         <v>150</v>
       </c>
@@ -2620,8 +2966,11 @@
       <c r="C113" t="s">
         <v>167</v>
       </c>
-    </row>
-    <row r="114" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D113" t="s">
+        <v>169</v>
+      </c>
+    </row>
+    <row r="114" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A114" t="s">
         <v>15</v>
       </c>
@@ -2631,8 +2980,11 @@
       <c r="C114" t="s">
         <v>166</v>
       </c>
-    </row>
-    <row r="115" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D114" t="s">
+        <v>169</v>
+      </c>
+    </row>
+    <row r="115" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A115" t="s">
         <v>155</v>
       </c>
@@ -2642,8 +2994,11 @@
       <c r="C115" t="s">
         <v>165</v>
       </c>
-    </row>
-    <row r="116" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D115" t="s">
+        <v>170</v>
+      </c>
+    </row>
+    <row r="116" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A116" t="s">
         <v>24</v>
       </c>
@@ -2653,8 +3008,11 @@
       <c r="C116" t="s">
         <v>165</v>
       </c>
-    </row>
-    <row r="117" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D116" t="s">
+        <v>170</v>
+      </c>
+    </row>
+    <row r="117" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A117" t="s">
         <v>97</v>
       </c>
@@ -2664,8 +3022,11 @@
       <c r="C117" t="s">
         <v>166</v>
       </c>
-    </row>
-    <row r="118" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D117" t="s">
+        <v>169</v>
+      </c>
+    </row>
+    <row r="118" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A118" t="s">
         <v>31</v>
       </c>
@@ -2675,8 +3036,11 @@
       <c r="C118" t="s">
         <v>167</v>
       </c>
-    </row>
-    <row r="119" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D118" t="s">
+        <v>169</v>
+      </c>
+    </row>
+    <row r="119" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A119" t="s">
         <v>127</v>
       </c>
@@ -2686,8 +3050,11 @@
       <c r="C119" t="s">
         <v>167</v>
       </c>
-    </row>
-    <row r="120" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D119" t="s">
+        <v>169</v>
+      </c>
+    </row>
+    <row r="120" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A120" t="s">
         <v>120</v>
       </c>
@@ -2697,8 +3064,11 @@
       <c r="C120" t="s">
         <v>167</v>
       </c>
-    </row>
-    <row r="121" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D120" t="s">
+        <v>169</v>
+      </c>
+    </row>
+    <row r="121" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A121" t="s">
         <v>126</v>
       </c>
@@ -2708,8 +3078,11 @@
       <c r="C121" t="s">
         <v>167</v>
       </c>
-    </row>
-    <row r="122" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D121" t="s">
+        <v>169</v>
+      </c>
+    </row>
+    <row r="122" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A122" t="s">
         <v>46</v>
       </c>
@@ -2719,8 +3092,11 @@
       <c r="C122" t="s">
         <v>167</v>
       </c>
-    </row>
-    <row r="123" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D122" t="s">
+        <v>169</v>
+      </c>
+    </row>
+    <row r="123" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A123" t="s">
         <v>90</v>
       </c>
@@ -2730,8 +3106,11 @@
       <c r="C123" t="s">
         <v>166</v>
       </c>
-    </row>
-    <row r="124" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D123" t="s">
+        <v>169</v>
+      </c>
+    </row>
+    <row r="124" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A124" t="s">
         <v>134</v>
       </c>
@@ -2741,8 +3120,11 @@
       <c r="C124" t="s">
         <v>165</v>
       </c>
-    </row>
-    <row r="125" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D124" t="s">
+        <v>170</v>
+      </c>
+    </row>
+    <row r="125" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A125" t="s">
         <v>29</v>
       </c>
@@ -2752,8 +3134,11 @@
       <c r="C125" t="s">
         <v>165</v>
       </c>
-    </row>
-    <row r="126" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D125" t="s">
+        <v>170</v>
+      </c>
+    </row>
+    <row r="126" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A126" t="s">
         <v>141</v>
       </c>
@@ -2763,8 +3148,11 @@
       <c r="C126" t="s">
         <v>166</v>
       </c>
-    </row>
-    <row r="127" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D126" t="s">
+        <v>169</v>
+      </c>
+    </row>
+    <row r="127" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A127" t="s">
         <v>139</v>
       </c>
@@ -2774,8 +3162,11 @@
       <c r="C127" t="s">
         <v>165</v>
       </c>
-    </row>
-    <row r="128" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D127" t="s">
+        <v>170</v>
+      </c>
+    </row>
+    <row r="128" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A128" t="s">
         <v>146</v>
       </c>
@@ -2785,8 +3176,11 @@
       <c r="C128" t="s">
         <v>165</v>
       </c>
-    </row>
-    <row r="129" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D128" t="s">
+        <v>170</v>
+      </c>
+    </row>
+    <row r="129" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A129" t="s">
         <v>14</v>
       </c>
@@ -2796,8 +3190,11 @@
       <c r="C129" t="s">
         <v>165</v>
       </c>
-    </row>
-    <row r="130" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D129" t="s">
+        <v>170</v>
+      </c>
+    </row>
+    <row r="130" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A130" t="s">
         <v>152</v>
       </c>
@@ -2807,8 +3204,11 @@
       <c r="C130" t="s">
         <v>165</v>
       </c>
-    </row>
-    <row r="131" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D130" t="s">
+        <v>170</v>
+      </c>
+    </row>
+    <row r="131" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A131" t="s">
         <v>11</v>
       </c>
@@ -2818,8 +3218,11 @@
       <c r="C131" t="s">
         <v>165</v>
       </c>
-    </row>
-    <row r="132" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D131" t="s">
+        <v>170</v>
+      </c>
+    </row>
+    <row r="132" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A132" t="s">
         <v>44</v>
       </c>
@@ -2829,8 +3232,11 @@
       <c r="C132" t="s">
         <v>165</v>
       </c>
-    </row>
-    <row r="133" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D132" t="s">
+        <v>170</v>
+      </c>
+    </row>
+    <row r="133" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A133" t="s">
         <v>62</v>
       </c>
@@ -2840,8 +3246,11 @@
       <c r="C133" t="s">
         <v>165</v>
       </c>
-    </row>
-    <row r="134" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D133" t="s">
+        <v>170</v>
+      </c>
+    </row>
+    <row r="134" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A134" t="s">
         <v>12</v>
       </c>
@@ -2851,8 +3260,11 @@
       <c r="C134" t="s">
         <v>165</v>
       </c>
-    </row>
-    <row r="135" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D134" t="s">
+        <v>170</v>
+      </c>
+    </row>
+    <row r="135" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A135" t="s">
         <v>148</v>
       </c>
@@ -2862,8 +3274,11 @@
       <c r="C135" t="s">
         <v>167</v>
       </c>
-    </row>
-    <row r="136" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D135" t="s">
+        <v>169</v>
+      </c>
+    </row>
+    <row r="136" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A136" t="s">
         <v>79</v>
       </c>
@@ -2873,8 +3288,11 @@
       <c r="C136" t="s">
         <v>167</v>
       </c>
-    </row>
-    <row r="137" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D136" t="s">
+        <v>169</v>
+      </c>
+    </row>
+    <row r="137" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A137" t="s">
         <v>18</v>
       </c>
@@ -2884,8 +3302,11 @@
       <c r="C137" t="s">
         <v>167</v>
       </c>
-    </row>
-    <row r="138" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D137" t="s">
+        <v>169</v>
+      </c>
+    </row>
+    <row r="138" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A138" t="s">
         <v>78</v>
       </c>
@@ -2895,8 +3316,11 @@
       <c r="C138" t="s">
         <v>167</v>
       </c>
-    </row>
-    <row r="139" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D138" t="s">
+        <v>169</v>
+      </c>
+    </row>
+    <row r="139" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A139" t="s">
         <v>117</v>
       </c>
@@ -2906,8 +3330,11 @@
       <c r="C139" t="s">
         <v>167</v>
       </c>
-    </row>
-    <row r="140" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D139" t="s">
+        <v>169</v>
+      </c>
+    </row>
+    <row r="140" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A140" t="s">
         <v>63</v>
       </c>
@@ -2917,8 +3344,11 @@
       <c r="C140" t="s">
         <v>165</v>
       </c>
-    </row>
-    <row r="141" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D140" t="s">
+        <v>170</v>
+      </c>
+    </row>
+    <row r="141" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A141" t="s">
         <v>45</v>
       </c>
@@ -2928,8 +3358,11 @@
       <c r="C141" t="s">
         <v>165</v>
       </c>
-    </row>
-    <row r="142" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D141" t="s">
+        <v>170</v>
+      </c>
+    </row>
+    <row r="142" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A142" t="s">
         <v>99</v>
       </c>
@@ -2939,8 +3372,11 @@
       <c r="C142" t="s">
         <v>167</v>
       </c>
-    </row>
-    <row r="143" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D142" t="s">
+        <v>169</v>
+      </c>
+    </row>
+    <row r="143" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A143" t="s">
         <v>66</v>
       </c>
@@ -2950,8 +3386,11 @@
       <c r="C143" t="s">
         <v>167</v>
       </c>
-    </row>
-    <row r="144" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D143" t="s">
+        <v>169</v>
+      </c>
+    </row>
+    <row r="144" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A144" t="s">
         <v>143</v>
       </c>
@@ -2961,8 +3400,11 @@
       <c r="C144" t="s">
         <v>167</v>
       </c>
-    </row>
-    <row r="145" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D144" t="s">
+        <v>169</v>
+      </c>
+    </row>
+    <row r="145" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A145" t="s">
         <v>153</v>
       </c>
@@ -2972,8 +3414,11 @@
       <c r="C145" t="s">
         <v>165</v>
       </c>
-    </row>
-    <row r="146" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D145" t="s">
+        <v>170</v>
+      </c>
+    </row>
+    <row r="146" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A146" t="s">
         <v>140</v>
       </c>
@@ -2983,8 +3428,11 @@
       <c r="C146" t="s">
         <v>166</v>
       </c>
-    </row>
-    <row r="147" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D146" t="s">
+        <v>169</v>
+      </c>
+    </row>
+    <row r="147" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A147" t="s">
         <v>159</v>
       </c>
@@ -2994,8 +3442,11 @@
       <c r="C147" t="s">
         <v>167</v>
       </c>
-    </row>
-    <row r="148" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D147" t="s">
+        <v>169</v>
+      </c>
+    </row>
+    <row r="148" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A148" t="s">
         <v>88</v>
       </c>
@@ -3005,8 +3456,11 @@
       <c r="C148" t="s">
         <v>167</v>
       </c>
-    </row>
-    <row r="149" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D148" t="s">
+        <v>169</v>
+      </c>
+    </row>
+    <row r="149" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A149" t="s">
         <v>142</v>
       </c>
@@ -3016,8 +3470,11 @@
       <c r="C149" t="s">
         <v>167</v>
       </c>
-    </row>
-    <row r="150" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D149" t="s">
+        <v>169</v>
+      </c>
+    </row>
+    <row r="150" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A150" t="s">
         <v>157</v>
       </c>
@@ -3027,8 +3484,11 @@
       <c r="C150" t="s">
         <v>165</v>
       </c>
-    </row>
-    <row r="151" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D150" t="s">
+        <v>170</v>
+      </c>
+    </row>
+    <row r="151" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A151" t="s">
         <v>118</v>
       </c>
@@ -3038,8 +3498,11 @@
       <c r="C151" t="s">
         <v>165</v>
       </c>
-    </row>
-    <row r="152" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D151" t="s">
+        <v>170</v>
+      </c>
+    </row>
+    <row r="152" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A152" t="s">
         <v>137</v>
       </c>
@@ -3049,8 +3512,11 @@
       <c r="C152" t="s">
         <v>166</v>
       </c>
-    </row>
-    <row r="153" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D152" t="s">
+        <v>169</v>
+      </c>
+    </row>
+    <row r="153" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A153" t="s">
         <v>72</v>
       </c>
@@ -3060,8 +3526,11 @@
       <c r="C153" t="s">
         <v>166</v>
       </c>
-    </row>
-    <row r="154" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D153" t="s">
+        <v>169</v>
+      </c>
+    </row>
+    <row r="154" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A154" t="s">
         <v>17</v>
       </c>
@@ -3071,8 +3540,11 @@
       <c r="C154" t="s">
         <v>166</v>
       </c>
-    </row>
-    <row r="155" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D154" t="s">
+        <v>169</v>
+      </c>
+    </row>
+    <row r="155" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A155" t="s">
         <v>93</v>
       </c>
@@ -3082,8 +3554,11 @@
       <c r="C155" t="s">
         <v>166</v>
       </c>
-    </row>
-    <row r="156" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D155" t="s">
+        <v>169</v>
+      </c>
+    </row>
+    <row r="156" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A156" t="s">
         <v>71</v>
       </c>
@@ -3093,8 +3568,11 @@
       <c r="C156" t="s">
         <v>167</v>
       </c>
-    </row>
-    <row r="157" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D156" t="s">
+        <v>169</v>
+      </c>
+    </row>
+    <row r="157" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A157" t="s">
         <v>128</v>
       </c>
@@ -3104,8 +3582,11 @@
       <c r="C157" t="s">
         <v>167</v>
       </c>
-    </row>
-    <row r="158" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D157" t="s">
+        <v>169</v>
+      </c>
+    </row>
+    <row r="158" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A158" t="s">
         <v>27</v>
       </c>
@@ -3115,8 +3596,11 @@
       <c r="C158" t="s">
         <v>167</v>
       </c>
-    </row>
-    <row r="159" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D158" t="s">
+        <v>169</v>
+      </c>
+    </row>
+    <row r="159" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A159" t="s">
         <v>149</v>
       </c>
@@ -3126,8 +3610,11 @@
       <c r="C159" t="s">
         <v>167</v>
       </c>
-    </row>
-    <row r="160" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D159" t="s">
+        <v>169</v>
+      </c>
+    </row>
+    <row r="160" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A160" t="s">
         <v>136</v>
       </c>
@@ -3137,8 +3624,11 @@
       <c r="C160" t="s">
         <v>167</v>
       </c>
-    </row>
-    <row r="161" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D160" t="s">
+        <v>169</v>
+      </c>
+    </row>
+    <row r="161" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A161" t="s">
         <v>110</v>
       </c>
@@ -3148,8 +3638,11 @@
       <c r="C161" t="s">
         <v>167</v>
       </c>
-    </row>
-    <row r="162" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D161" t="s">
+        <v>169</v>
+      </c>
+    </row>
+    <row r="162" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A162" t="s">
         <v>9</v>
       </c>
@@ -3159,13 +3652,12 @@
       <c r="C162" t="s">
         <v>167</v>
       </c>
+      <c r="D162" t="s">
+        <v>169</v>
+      </c>
     </row>
   </sheetData>
-  <autoFilter ref="A1:C162" xr:uid="{C0794E99-E09B-284B-B1A7-A3DBFFA417DB}">
-    <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:C162">
-      <sortCondition ref="A1:A162"/>
-    </sortState>
-  </autoFilter>
+  <autoFilter ref="A1:D162" xr:uid="{DD2EE166-89C9-3443-922F-28400AF0BA12}"/>
   <pageMargins left="0.78740157499999996" right="0.78740157499999996" top="0.984251969" bottom="0.984251969" header="0.4921259845" footer="0.4921259845"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
final dataset --> final.csv
</commit_message>
<xml_diff>
--- a/01_input/swiss_teams_lamguage.xlsx
+++ b/01_input/swiss_teams_lamguage.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10810"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11108"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/nicowyss/Documents/Git/social_analysis_football_transfer/01_input/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/kosta/Documents/01_HSLU/03.Semester/Analysis_of_social_interactions/Group/Github_AMS/social_analysis_football_transfer/01_input/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{523D3387-C37B-9647-B05B-69BD5FD22230}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E2B60A6B-58F2-F24B-8179-659513B1E413}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-20" yWindow="520" windowWidth="33600" windowHeight="20500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="20" yWindow="460" windowWidth="28800" windowHeight="16420" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="swiss_teams_lamguage" sheetId="1" r:id="rId1"/>
@@ -511,15 +511,6 @@
     <t>Azzurri LS</t>
   </si>
   <si>
-    <t>Club</t>
-  </si>
-  <si>
-    <t>Land</t>
-  </si>
-  <si>
-    <t>Sprache</t>
-  </si>
-  <si>
     <t>German</t>
   </si>
   <si>
@@ -529,13 +520,22 @@
     <t>French</t>
   </si>
   <si>
-    <t>Language Familiy</t>
-  </si>
-  <si>
     <t>Romance</t>
   </si>
   <si>
     <t>Germanic</t>
+  </si>
+  <si>
+    <t>Team</t>
+  </si>
+  <si>
+    <t>Country</t>
+  </si>
+  <si>
+    <t>Language</t>
+  </si>
+  <si>
+    <t>LanguageFamily</t>
   </si>
 </sst>
 </file>
@@ -1378,28 +1378,26 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:D162"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="J23" sqref="J23"/>
-    </sheetView>
+    <sheetView tabSelected="1" zoomScale="125" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="33.5" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="15.5" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="20.5" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
-        <v>162</v>
+        <v>167</v>
       </c>
       <c r="B1" t="s">
-        <v>163</v>
+        <v>168</v>
       </c>
       <c r="C1" t="s">
-        <v>164</v>
+        <v>169</v>
       </c>
       <c r="D1" t="s">
-        <v>168</v>
+        <v>170</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.2">
@@ -1410,10 +1408,10 @@
         <v>1</v>
       </c>
       <c r="C2" t="s">
-        <v>166</v>
+        <v>163</v>
       </c>
       <c r="D2" t="s">
-        <v>169</v>
+        <v>165</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.2">
@@ -1424,10 +1422,10 @@
         <v>1</v>
       </c>
       <c r="C3" t="s">
-        <v>165</v>
+        <v>162</v>
       </c>
       <c r="D3" t="s">
-        <v>170</v>
+        <v>166</v>
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.2">
@@ -1438,10 +1436,10 @@
         <v>1</v>
       </c>
       <c r="C4" t="s">
-        <v>165</v>
+        <v>162</v>
       </c>
       <c r="D4" t="s">
-        <v>170</v>
+        <v>166</v>
       </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.2">
@@ -1452,10 +1450,10 @@
         <v>1</v>
       </c>
       <c r="C5" t="s">
-        <v>165</v>
+        <v>162</v>
       </c>
       <c r="D5" t="s">
-        <v>170</v>
+        <v>166</v>
       </c>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.2">
@@ -1466,10 +1464,10 @@
         <v>1</v>
       </c>
       <c r="C6" t="s">
-        <v>166</v>
+        <v>163</v>
       </c>
       <c r="D6" t="s">
-        <v>169</v>
+        <v>165</v>
       </c>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.2">
@@ -1480,10 +1478,10 @@
         <v>1</v>
       </c>
       <c r="C7" t="s">
-        <v>166</v>
+        <v>163</v>
       </c>
       <c r="D7" t="s">
-        <v>169</v>
+        <v>165</v>
       </c>
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.2">
@@ -1494,10 +1492,10 @@
         <v>1</v>
       </c>
       <c r="C8" t="s">
-        <v>166</v>
+        <v>163</v>
       </c>
       <c r="D8" t="s">
-        <v>169</v>
+        <v>165</v>
       </c>
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.2">
@@ -1508,10 +1506,10 @@
         <v>1</v>
       </c>
       <c r="C9" t="s">
-        <v>166</v>
+        <v>163</v>
       </c>
       <c r="D9" t="s">
-        <v>169</v>
+        <v>165</v>
       </c>
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.2">
@@ -1522,10 +1520,10 @@
         <v>1</v>
       </c>
       <c r="C10" t="s">
-        <v>166</v>
+        <v>163</v>
       </c>
       <c r="D10" t="s">
-        <v>169</v>
+        <v>165</v>
       </c>
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.2">
@@ -1536,10 +1534,10 @@
         <v>1</v>
       </c>
       <c r="C11" t="s">
-        <v>166</v>
+        <v>163</v>
       </c>
       <c r="D11" t="s">
-        <v>169</v>
+        <v>165</v>
       </c>
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.2">
@@ -1550,10 +1548,10 @@
         <v>1</v>
       </c>
       <c r="C12" t="s">
-        <v>166</v>
+        <v>163</v>
       </c>
       <c r="D12" t="s">
-        <v>169</v>
+        <v>165</v>
       </c>
     </row>
     <row r="13" spans="1:4" x14ac:dyDescent="0.2">
@@ -1564,10 +1562,10 @@
         <v>1</v>
       </c>
       <c r="C13" t="s">
-        <v>166</v>
+        <v>163</v>
       </c>
       <c r="D13" t="s">
-        <v>169</v>
+        <v>165</v>
       </c>
     </row>
     <row r="14" spans="1:4" x14ac:dyDescent="0.2">
@@ -1578,10 +1576,10 @@
         <v>1</v>
       </c>
       <c r="C14" t="s">
-        <v>166</v>
+        <v>163</v>
       </c>
       <c r="D14" t="s">
-        <v>169</v>
+        <v>165</v>
       </c>
     </row>
     <row r="15" spans="1:4" x14ac:dyDescent="0.2">
@@ -1592,10 +1590,10 @@
         <v>1</v>
       </c>
       <c r="C15" t="s">
-        <v>166</v>
+        <v>163</v>
       </c>
       <c r="D15" t="s">
-        <v>169</v>
+        <v>165</v>
       </c>
     </row>
     <row r="16" spans="1:4" x14ac:dyDescent="0.2">
@@ -1606,10 +1604,10 @@
         <v>1</v>
       </c>
       <c r="C16" t="s">
-        <v>166</v>
+        <v>163</v>
       </c>
       <c r="D16" t="s">
-        <v>169</v>
+        <v>165</v>
       </c>
     </row>
     <row r="17" spans="1:4" x14ac:dyDescent="0.2">
@@ -1620,10 +1618,10 @@
         <v>1</v>
       </c>
       <c r="C17" t="s">
-        <v>166</v>
+        <v>163</v>
       </c>
       <c r="D17" t="s">
-        <v>169</v>
+        <v>165</v>
       </c>
     </row>
     <row r="18" spans="1:4" x14ac:dyDescent="0.2">
@@ -1634,10 +1632,10 @@
         <v>1</v>
       </c>
       <c r="C18" t="s">
-        <v>165</v>
+        <v>162</v>
       </c>
       <c r="D18" t="s">
-        <v>170</v>
+        <v>166</v>
       </c>
     </row>
     <row r="19" spans="1:4" x14ac:dyDescent="0.2">
@@ -1648,10 +1646,10 @@
         <v>1</v>
       </c>
       <c r="C19" t="s">
-        <v>165</v>
+        <v>162</v>
       </c>
       <c r="D19" t="s">
-        <v>170</v>
+        <v>166</v>
       </c>
     </row>
     <row r="20" spans="1:4" x14ac:dyDescent="0.2">
@@ -1662,10 +1660,10 @@
         <v>1</v>
       </c>
       <c r="C20" t="s">
-        <v>165</v>
+        <v>162</v>
       </c>
       <c r="D20" t="s">
-        <v>170</v>
+        <v>166</v>
       </c>
     </row>
     <row r="21" spans="1:4" x14ac:dyDescent="0.2">
@@ -1676,10 +1674,10 @@
         <v>1</v>
       </c>
       <c r="C21" t="s">
-        <v>165</v>
+        <v>162</v>
       </c>
       <c r="D21" t="s">
-        <v>170</v>
+        <v>166</v>
       </c>
     </row>
     <row r="22" spans="1:4" x14ac:dyDescent="0.2">
@@ -1690,10 +1688,10 @@
         <v>1</v>
       </c>
       <c r="C22" t="s">
-        <v>167</v>
+        <v>164</v>
       </c>
       <c r="D22" t="s">
-        <v>169</v>
+        <v>165</v>
       </c>
     </row>
     <row r="23" spans="1:4" x14ac:dyDescent="0.2">
@@ -1704,10 +1702,10 @@
         <v>1</v>
       </c>
       <c r="C23" t="s">
-        <v>165</v>
+        <v>162</v>
       </c>
       <c r="D23" t="s">
-        <v>170</v>
+        <v>166</v>
       </c>
     </row>
     <row r="24" spans="1:4" x14ac:dyDescent="0.2">
@@ -1718,10 +1716,10 @@
         <v>1</v>
       </c>
       <c r="C24" t="s">
-        <v>167</v>
+        <v>164</v>
       </c>
       <c r="D24" t="s">
-        <v>169</v>
+        <v>165</v>
       </c>
     </row>
     <row r="25" spans="1:4" x14ac:dyDescent="0.2">
@@ -1732,10 +1730,10 @@
         <v>1</v>
       </c>
       <c r="C25" t="s">
-        <v>165</v>
+        <v>162</v>
       </c>
       <c r="D25" t="s">
-        <v>170</v>
+        <v>166</v>
       </c>
     </row>
     <row r="26" spans="1:4" x14ac:dyDescent="0.2">
@@ -1746,10 +1744,10 @@
         <v>1</v>
       </c>
       <c r="C26" t="s">
-        <v>167</v>
+        <v>164</v>
       </c>
       <c r="D26" t="s">
-        <v>169</v>
+        <v>165</v>
       </c>
     </row>
     <row r="27" spans="1:4" x14ac:dyDescent="0.2">
@@ -1760,10 +1758,10 @@
         <v>1</v>
       </c>
       <c r="C27" t="s">
-        <v>165</v>
+        <v>162</v>
       </c>
       <c r="D27" t="s">
-        <v>170</v>
+        <v>166</v>
       </c>
     </row>
     <row r="28" spans="1:4" x14ac:dyDescent="0.2">
@@ -1774,10 +1772,10 @@
         <v>1</v>
       </c>
       <c r="C28" t="s">
-        <v>165</v>
+        <v>162</v>
       </c>
       <c r="D28" t="s">
-        <v>170</v>
+        <v>166</v>
       </c>
     </row>
     <row r="29" spans="1:4" x14ac:dyDescent="0.2">
@@ -1788,10 +1786,10 @@
         <v>1</v>
       </c>
       <c r="C29" t="s">
-        <v>165</v>
+        <v>162</v>
       </c>
       <c r="D29" t="s">
-        <v>170</v>
+        <v>166</v>
       </c>
     </row>
     <row r="30" spans="1:4" x14ac:dyDescent="0.2">
@@ -1802,10 +1800,10 @@
         <v>1</v>
       </c>
       <c r="C30" t="s">
-        <v>167</v>
+        <v>164</v>
       </c>
       <c r="D30" t="s">
-        <v>169</v>
+        <v>165</v>
       </c>
     </row>
     <row r="31" spans="1:4" x14ac:dyDescent="0.2">
@@ -1816,10 +1814,10 @@
         <v>1</v>
       </c>
       <c r="C31" t="s">
-        <v>167</v>
+        <v>164</v>
       </c>
       <c r="D31" t="s">
-        <v>169</v>
+        <v>165</v>
       </c>
     </row>
     <row r="32" spans="1:4" x14ac:dyDescent="0.2">
@@ -1830,10 +1828,10 @@
         <v>1</v>
       </c>
       <c r="C32" t="s">
-        <v>166</v>
+        <v>163</v>
       </c>
       <c r="D32" t="s">
-        <v>169</v>
+        <v>165</v>
       </c>
     </row>
     <row r="33" spans="1:4" x14ac:dyDescent="0.2">
@@ -1844,10 +1842,10 @@
         <v>1</v>
       </c>
       <c r="C33" t="s">
-        <v>165</v>
+        <v>162</v>
       </c>
       <c r="D33" t="s">
-        <v>170</v>
+        <v>166</v>
       </c>
     </row>
     <row r="34" spans="1:4" x14ac:dyDescent="0.2">
@@ -1858,10 +1856,10 @@
         <v>1</v>
       </c>
       <c r="C34" t="s">
-        <v>165</v>
+        <v>162</v>
       </c>
       <c r="D34" t="s">
-        <v>170</v>
+        <v>166</v>
       </c>
     </row>
     <row r="35" spans="1:4" x14ac:dyDescent="0.2">
@@ -1872,10 +1870,10 @@
         <v>1</v>
       </c>
       <c r="C35" t="s">
-        <v>165</v>
+        <v>162</v>
       </c>
       <c r="D35" t="s">
-        <v>170</v>
+        <v>166</v>
       </c>
     </row>
     <row r="36" spans="1:4" x14ac:dyDescent="0.2">
@@ -1886,10 +1884,10 @@
         <v>1</v>
       </c>
       <c r="C36" t="s">
-        <v>165</v>
+        <v>162</v>
       </c>
       <c r="D36" t="s">
-        <v>170</v>
+        <v>166</v>
       </c>
     </row>
     <row r="37" spans="1:4" x14ac:dyDescent="0.2">
@@ -1900,10 +1898,10 @@
         <v>1</v>
       </c>
       <c r="C37" t="s">
-        <v>165</v>
+        <v>162</v>
       </c>
       <c r="D37" t="s">
-        <v>170</v>
+        <v>166</v>
       </c>
     </row>
     <row r="38" spans="1:4" x14ac:dyDescent="0.2">
@@ -1914,10 +1912,10 @@
         <v>1</v>
       </c>
       <c r="C38" t="s">
-        <v>165</v>
+        <v>162</v>
       </c>
       <c r="D38" t="s">
-        <v>170</v>
+        <v>166</v>
       </c>
     </row>
     <row r="39" spans="1:4" x14ac:dyDescent="0.2">
@@ -1928,10 +1926,10 @@
         <v>1</v>
       </c>
       <c r="C39" t="s">
-        <v>167</v>
+        <v>164</v>
       </c>
       <c r="D39" t="s">
-        <v>169</v>
+        <v>165</v>
       </c>
     </row>
     <row r="40" spans="1:4" x14ac:dyDescent="0.2">
@@ -1942,10 +1940,10 @@
         <v>1</v>
       </c>
       <c r="C40" t="s">
-        <v>167</v>
+        <v>164</v>
       </c>
       <c r="D40" t="s">
-        <v>169</v>
+        <v>165</v>
       </c>
     </row>
     <row r="41" spans="1:4" x14ac:dyDescent="0.2">
@@ -1956,10 +1954,10 @@
         <v>1</v>
       </c>
       <c r="C41" t="s">
-        <v>167</v>
+        <v>164</v>
       </c>
       <c r="D41" t="s">
-        <v>169</v>
+        <v>165</v>
       </c>
     </row>
     <row r="42" spans="1:4" x14ac:dyDescent="0.2">
@@ -1970,10 +1968,10 @@
         <v>1</v>
       </c>
       <c r="C42" t="s">
-        <v>165</v>
+        <v>162</v>
       </c>
       <c r="D42" t="s">
-        <v>170</v>
+        <v>166</v>
       </c>
     </row>
     <row r="43" spans="1:4" x14ac:dyDescent="0.2">
@@ -1984,10 +1982,10 @@
         <v>1</v>
       </c>
       <c r="C43" t="s">
-        <v>165</v>
+        <v>162</v>
       </c>
       <c r="D43" t="s">
-        <v>170</v>
+        <v>166</v>
       </c>
     </row>
     <row r="44" spans="1:4" x14ac:dyDescent="0.2">
@@ -1998,10 +1996,10 @@
         <v>1</v>
       </c>
       <c r="C44" t="s">
-        <v>165</v>
+        <v>162</v>
       </c>
       <c r="D44" t="s">
-        <v>170</v>
+        <v>166</v>
       </c>
     </row>
     <row r="45" spans="1:4" x14ac:dyDescent="0.2">
@@ -2012,10 +2010,10 @@
         <v>1</v>
       </c>
       <c r="C45" t="s">
-        <v>166</v>
+        <v>163</v>
       </c>
       <c r="D45" t="s">
-        <v>169</v>
+        <v>165</v>
       </c>
     </row>
     <row r="46" spans="1:4" x14ac:dyDescent="0.2">
@@ -2026,10 +2024,10 @@
         <v>1</v>
       </c>
       <c r="C46" t="s">
-        <v>166</v>
+        <v>163</v>
       </c>
       <c r="D46" t="s">
-        <v>169</v>
+        <v>165</v>
       </c>
     </row>
     <row r="47" spans="1:4" x14ac:dyDescent="0.2">
@@ -2040,10 +2038,10 @@
         <v>1</v>
       </c>
       <c r="C47" t="s">
-        <v>167</v>
+        <v>164</v>
       </c>
       <c r="D47" t="s">
-        <v>169</v>
+        <v>165</v>
       </c>
     </row>
     <row r="48" spans="1:4" x14ac:dyDescent="0.2">
@@ -2054,10 +2052,10 @@
         <v>1</v>
       </c>
       <c r="C48" t="s">
-        <v>167</v>
+        <v>164</v>
       </c>
       <c r="D48" t="s">
-        <v>169</v>
+        <v>165</v>
       </c>
     </row>
     <row r="49" spans="1:4" x14ac:dyDescent="0.2">
@@ -2068,10 +2066,10 @@
         <v>1</v>
       </c>
       <c r="C49" t="s">
-        <v>165</v>
+        <v>162</v>
       </c>
       <c r="D49" t="s">
-        <v>170</v>
+        <v>166</v>
       </c>
     </row>
     <row r="50" spans="1:4" x14ac:dyDescent="0.2">
@@ -2082,10 +2080,10 @@
         <v>1</v>
       </c>
       <c r="C50" t="s">
-        <v>165</v>
+        <v>162</v>
       </c>
       <c r="D50" t="s">
-        <v>170</v>
+        <v>166</v>
       </c>
     </row>
     <row r="51" spans="1:4" x14ac:dyDescent="0.2">
@@ -2096,10 +2094,10 @@
         <v>1</v>
       </c>
       <c r="C51" t="s">
-        <v>167</v>
+        <v>164</v>
       </c>
       <c r="D51" t="s">
-        <v>169</v>
+        <v>165</v>
       </c>
     </row>
     <row r="52" spans="1:4" x14ac:dyDescent="0.2">
@@ -2110,10 +2108,10 @@
         <v>1</v>
       </c>
       <c r="C52" t="s">
-        <v>165</v>
+        <v>162</v>
       </c>
       <c r="D52" t="s">
-        <v>170</v>
+        <v>166</v>
       </c>
     </row>
     <row r="53" spans="1:4" x14ac:dyDescent="0.2">
@@ -2124,10 +2122,10 @@
         <v>1</v>
       </c>
       <c r="C53" t="s">
-        <v>165</v>
+        <v>162</v>
       </c>
       <c r="D53" t="s">
-        <v>170</v>
+        <v>166</v>
       </c>
     </row>
     <row r="54" spans="1:4" x14ac:dyDescent="0.2">
@@ -2138,10 +2136,10 @@
         <v>1</v>
       </c>
       <c r="C54" t="s">
-        <v>167</v>
+        <v>164</v>
       </c>
       <c r="D54" t="s">
-        <v>169</v>
+        <v>165</v>
       </c>
     </row>
     <row r="55" spans="1:4" x14ac:dyDescent="0.2">
@@ -2152,10 +2150,10 @@
         <v>1</v>
       </c>
       <c r="C55" t="s">
-        <v>165</v>
+        <v>162</v>
       </c>
       <c r="D55" t="s">
-        <v>170</v>
+        <v>166</v>
       </c>
     </row>
     <row r="56" spans="1:4" x14ac:dyDescent="0.2">
@@ -2166,10 +2164,10 @@
         <v>1</v>
       </c>
       <c r="C56" t="s">
-        <v>167</v>
+        <v>164</v>
       </c>
       <c r="D56" t="s">
-        <v>169</v>
+        <v>165</v>
       </c>
     </row>
     <row r="57" spans="1:4" x14ac:dyDescent="0.2">
@@ -2180,10 +2178,10 @@
         <v>1</v>
       </c>
       <c r="C57" t="s">
-        <v>166</v>
+        <v>163</v>
       </c>
       <c r="D57" t="s">
-        <v>169</v>
+        <v>165</v>
       </c>
     </row>
     <row r="58" spans="1:4" x14ac:dyDescent="0.2">
@@ -2194,10 +2192,10 @@
         <v>1</v>
       </c>
       <c r="C58" t="s">
-        <v>165</v>
+        <v>162</v>
       </c>
       <c r="D58" t="s">
-        <v>170</v>
+        <v>166</v>
       </c>
     </row>
     <row r="59" spans="1:4" x14ac:dyDescent="0.2">
@@ -2208,10 +2206,10 @@
         <v>1</v>
       </c>
       <c r="C59" t="s">
-        <v>165</v>
+        <v>162</v>
       </c>
       <c r="D59" t="s">
-        <v>170</v>
+        <v>166</v>
       </c>
     </row>
     <row r="60" spans="1:4" x14ac:dyDescent="0.2">
@@ -2222,10 +2220,10 @@
         <v>1</v>
       </c>
       <c r="C60" t="s">
-        <v>165</v>
+        <v>162</v>
       </c>
       <c r="D60" t="s">
-        <v>170</v>
+        <v>166</v>
       </c>
     </row>
     <row r="61" spans="1:4" x14ac:dyDescent="0.2">
@@ -2236,10 +2234,10 @@
         <v>1</v>
       </c>
       <c r="C61" t="s">
-        <v>165</v>
+        <v>162</v>
       </c>
       <c r="D61" t="s">
-        <v>170</v>
+        <v>166</v>
       </c>
     </row>
     <row r="62" spans="1:4" x14ac:dyDescent="0.2">
@@ -2250,10 +2248,10 @@
         <v>1</v>
       </c>
       <c r="C62" t="s">
-        <v>167</v>
+        <v>164</v>
       </c>
       <c r="D62" t="s">
-        <v>169</v>
+        <v>165</v>
       </c>
     </row>
     <row r="63" spans="1:4" x14ac:dyDescent="0.2">
@@ -2264,10 +2262,10 @@
         <v>1</v>
       </c>
       <c r="C63" t="s">
-        <v>165</v>
+        <v>162</v>
       </c>
       <c r="D63" t="s">
-        <v>170</v>
+        <v>166</v>
       </c>
     </row>
     <row r="64" spans="1:4" x14ac:dyDescent="0.2">
@@ -2278,10 +2276,10 @@
         <v>1</v>
       </c>
       <c r="C64" t="s">
-        <v>165</v>
+        <v>162</v>
       </c>
       <c r="D64" t="s">
-        <v>170</v>
+        <v>166</v>
       </c>
     </row>
     <row r="65" spans="1:4" x14ac:dyDescent="0.2">
@@ -2292,10 +2290,10 @@
         <v>1</v>
       </c>
       <c r="C65" t="s">
-        <v>166</v>
+        <v>163</v>
       </c>
       <c r="D65" t="s">
-        <v>169</v>
+        <v>165</v>
       </c>
     </row>
     <row r="66" spans="1:4" x14ac:dyDescent="0.2">
@@ -2306,10 +2304,10 @@
         <v>1</v>
       </c>
       <c r="C66" t="s">
-        <v>166</v>
+        <v>163</v>
       </c>
       <c r="D66" t="s">
-        <v>169</v>
+        <v>165</v>
       </c>
     </row>
     <row r="67" spans="1:4" x14ac:dyDescent="0.2">
@@ -2320,10 +2318,10 @@
         <v>1</v>
       </c>
       <c r="C67" t="s">
-        <v>166</v>
+        <v>163</v>
       </c>
       <c r="D67" t="s">
-        <v>169</v>
+        <v>165</v>
       </c>
     </row>
     <row r="68" spans="1:4" x14ac:dyDescent="0.2">
@@ -2334,10 +2332,10 @@
         <v>1</v>
       </c>
       <c r="C68" t="s">
-        <v>165</v>
+        <v>162</v>
       </c>
       <c r="D68" t="s">
-        <v>170</v>
+        <v>166</v>
       </c>
     </row>
     <row r="69" spans="1:4" x14ac:dyDescent="0.2">
@@ -2348,10 +2346,10 @@
         <v>1</v>
       </c>
       <c r="C69" t="s">
-        <v>166</v>
+        <v>163</v>
       </c>
       <c r="D69" t="s">
-        <v>169</v>
+        <v>165</v>
       </c>
     </row>
     <row r="70" spans="1:4" x14ac:dyDescent="0.2">
@@ -2362,10 +2360,10 @@
         <v>1</v>
       </c>
       <c r="C70" t="s">
-        <v>166</v>
+        <v>163</v>
       </c>
       <c r="D70" t="s">
-        <v>169</v>
+        <v>165</v>
       </c>
     </row>
     <row r="71" spans="1:4" x14ac:dyDescent="0.2">
@@ -2376,10 +2374,10 @@
         <v>1</v>
       </c>
       <c r="C71" t="s">
-        <v>167</v>
+        <v>164</v>
       </c>
       <c r="D71" t="s">
-        <v>169</v>
+        <v>165</v>
       </c>
     </row>
     <row r="72" spans="1:4" x14ac:dyDescent="0.2">
@@ -2390,10 +2388,10 @@
         <v>1</v>
       </c>
       <c r="C72" t="s">
-        <v>165</v>
+        <v>162</v>
       </c>
       <c r="D72" t="s">
-        <v>170</v>
+        <v>166</v>
       </c>
     </row>
     <row r="73" spans="1:4" x14ac:dyDescent="0.2">
@@ -2404,10 +2402,10 @@
         <v>1</v>
       </c>
       <c r="C73" t="s">
-        <v>165</v>
+        <v>162</v>
       </c>
       <c r="D73" t="s">
-        <v>170</v>
+        <v>166</v>
       </c>
     </row>
     <row r="74" spans="1:4" x14ac:dyDescent="0.2">
@@ -2418,10 +2416,10 @@
         <v>1</v>
       </c>
       <c r="C74" t="s">
-        <v>165</v>
+        <v>162</v>
       </c>
       <c r="D74" t="s">
-        <v>170</v>
+        <v>166</v>
       </c>
     </row>
     <row r="75" spans="1:4" x14ac:dyDescent="0.2">
@@ -2432,10 +2430,10 @@
         <v>1</v>
       </c>
       <c r="C75" t="s">
-        <v>166</v>
+        <v>163</v>
       </c>
       <c r="D75" t="s">
-        <v>169</v>
+        <v>165</v>
       </c>
     </row>
     <row r="76" spans="1:4" x14ac:dyDescent="0.2">
@@ -2446,10 +2444,10 @@
         <v>1</v>
       </c>
       <c r="C76" t="s">
-        <v>167</v>
+        <v>164</v>
       </c>
       <c r="D76" t="s">
-        <v>169</v>
+        <v>165</v>
       </c>
     </row>
     <row r="77" spans="1:4" x14ac:dyDescent="0.2">
@@ -2460,10 +2458,10 @@
         <v>1</v>
       </c>
       <c r="C77" t="s">
-        <v>166</v>
+        <v>163</v>
       </c>
       <c r="D77" t="s">
-        <v>169</v>
+        <v>165</v>
       </c>
     </row>
     <row r="78" spans="1:4" x14ac:dyDescent="0.2">
@@ -2474,10 +2472,10 @@
         <v>1</v>
       </c>
       <c r="C78" t="s">
-        <v>167</v>
+        <v>164</v>
       </c>
       <c r="D78" t="s">
-        <v>169</v>
+        <v>165</v>
       </c>
     </row>
     <row r="79" spans="1:4" x14ac:dyDescent="0.2">
@@ -2488,10 +2486,10 @@
         <v>1</v>
       </c>
       <c r="C79" t="s">
-        <v>165</v>
+        <v>162</v>
       </c>
       <c r="D79" t="s">
-        <v>170</v>
+        <v>166</v>
       </c>
     </row>
     <row r="80" spans="1:4" x14ac:dyDescent="0.2">
@@ -2502,10 +2500,10 @@
         <v>1</v>
       </c>
       <c r="C80" t="s">
-        <v>165</v>
+        <v>162</v>
       </c>
       <c r="D80" t="s">
-        <v>170</v>
+        <v>166</v>
       </c>
     </row>
     <row r="81" spans="1:4" x14ac:dyDescent="0.2">
@@ -2516,10 +2514,10 @@
         <v>1</v>
       </c>
       <c r="C81" t="s">
-        <v>167</v>
+        <v>164</v>
       </c>
       <c r="D81" t="s">
-        <v>169</v>
+        <v>165</v>
       </c>
     </row>
     <row r="82" spans="1:4" x14ac:dyDescent="0.2">
@@ -2530,10 +2528,10 @@
         <v>1</v>
       </c>
       <c r="C82" t="s">
-        <v>167</v>
+        <v>164</v>
       </c>
       <c r="D82" t="s">
-        <v>169</v>
+        <v>165</v>
       </c>
     </row>
     <row r="83" spans="1:4" x14ac:dyDescent="0.2">
@@ -2544,10 +2542,10 @@
         <v>1</v>
       </c>
       <c r="C83" t="s">
-        <v>167</v>
+        <v>164</v>
       </c>
       <c r="D83" t="s">
-        <v>169</v>
+        <v>165</v>
       </c>
     </row>
     <row r="84" spans="1:4" x14ac:dyDescent="0.2">
@@ -2558,10 +2556,10 @@
         <v>1</v>
       </c>
       <c r="C84" t="s">
-        <v>167</v>
+        <v>164</v>
       </c>
       <c r="D84" t="s">
-        <v>169</v>
+        <v>165</v>
       </c>
     </row>
     <row r="85" spans="1:4" x14ac:dyDescent="0.2">
@@ -2572,10 +2570,10 @@
         <v>1</v>
       </c>
       <c r="C85" t="s">
-        <v>167</v>
+        <v>164</v>
       </c>
       <c r="D85" t="s">
-        <v>169</v>
+        <v>165</v>
       </c>
     </row>
     <row r="86" spans="1:4" x14ac:dyDescent="0.2">
@@ -2586,10 +2584,10 @@
         <v>1</v>
       </c>
       <c r="C86" t="s">
-        <v>165</v>
+        <v>162</v>
       </c>
       <c r="D86" t="s">
-        <v>170</v>
+        <v>166</v>
       </c>
     </row>
     <row r="87" spans="1:4" x14ac:dyDescent="0.2">
@@ -2600,10 +2598,10 @@
         <v>1</v>
       </c>
       <c r="C87" t="s">
-        <v>165</v>
+        <v>162</v>
       </c>
       <c r="D87" t="s">
-        <v>170</v>
+        <v>166</v>
       </c>
     </row>
     <row r="88" spans="1:4" x14ac:dyDescent="0.2">
@@ -2614,10 +2612,10 @@
         <v>1</v>
       </c>
       <c r="C88" t="s">
-        <v>165</v>
+        <v>162</v>
       </c>
       <c r="D88" t="s">
-        <v>170</v>
+        <v>166</v>
       </c>
     </row>
     <row r="89" spans="1:4" x14ac:dyDescent="0.2">
@@ -2628,10 +2626,10 @@
         <v>1</v>
       </c>
       <c r="C89" t="s">
-        <v>165</v>
+        <v>162</v>
       </c>
       <c r="D89" t="s">
-        <v>170</v>
+        <v>166</v>
       </c>
     </row>
     <row r="90" spans="1:4" x14ac:dyDescent="0.2">
@@ -2642,10 +2640,10 @@
         <v>1</v>
       </c>
       <c r="C90" t="s">
-        <v>165</v>
+        <v>162</v>
       </c>
       <c r="D90" t="s">
-        <v>170</v>
+        <v>166</v>
       </c>
     </row>
     <row r="91" spans="1:4" x14ac:dyDescent="0.2">
@@ -2656,10 +2654,10 @@
         <v>1</v>
       </c>
       <c r="C91" t="s">
-        <v>165</v>
+        <v>162</v>
       </c>
       <c r="D91" t="s">
-        <v>170</v>
+        <v>166</v>
       </c>
     </row>
     <row r="92" spans="1:4" x14ac:dyDescent="0.2">
@@ -2670,10 +2668,10 @@
         <v>1</v>
       </c>
       <c r="C92" t="s">
-        <v>165</v>
+        <v>162</v>
       </c>
       <c r="D92" t="s">
-        <v>170</v>
+        <v>166</v>
       </c>
     </row>
     <row r="93" spans="1:4" x14ac:dyDescent="0.2">
@@ -2684,10 +2682,10 @@
         <v>1</v>
       </c>
       <c r="C93" t="s">
-        <v>165</v>
+        <v>162</v>
       </c>
       <c r="D93" t="s">
-        <v>170</v>
+        <v>166</v>
       </c>
     </row>
     <row r="94" spans="1:4" x14ac:dyDescent="0.2">
@@ -2698,10 +2696,10 @@
         <v>1</v>
       </c>
       <c r="C94" t="s">
-        <v>165</v>
+        <v>162</v>
       </c>
       <c r="D94" t="s">
-        <v>170</v>
+        <v>166</v>
       </c>
     </row>
     <row r="95" spans="1:4" x14ac:dyDescent="0.2">
@@ -2712,10 +2710,10 @@
         <v>1</v>
       </c>
       <c r="C95" t="s">
-        <v>165</v>
+        <v>162</v>
       </c>
       <c r="D95" t="s">
-        <v>170</v>
+        <v>166</v>
       </c>
     </row>
     <row r="96" spans="1:4" x14ac:dyDescent="0.2">
@@ -2726,10 +2724,10 @@
         <v>1</v>
       </c>
       <c r="C96" t="s">
-        <v>165</v>
+        <v>162</v>
       </c>
       <c r="D96" t="s">
-        <v>170</v>
+        <v>166</v>
       </c>
     </row>
     <row r="97" spans="1:4" x14ac:dyDescent="0.2">
@@ -2740,10 +2738,10 @@
         <v>1</v>
       </c>
       <c r="C97" t="s">
-        <v>165</v>
+        <v>162</v>
       </c>
       <c r="D97" t="s">
-        <v>170</v>
+        <v>166</v>
       </c>
     </row>
     <row r="98" spans="1:4" x14ac:dyDescent="0.2">
@@ -2754,10 +2752,10 @@
         <v>1</v>
       </c>
       <c r="C98" t="s">
-        <v>165</v>
+        <v>162</v>
       </c>
       <c r="D98" t="s">
-        <v>170</v>
+        <v>166</v>
       </c>
     </row>
     <row r="99" spans="1:4" x14ac:dyDescent="0.2">
@@ -2768,10 +2766,10 @@
         <v>1</v>
       </c>
       <c r="C99" t="s">
-        <v>165</v>
+        <v>162</v>
       </c>
       <c r="D99" t="s">
-        <v>170</v>
+        <v>166</v>
       </c>
     </row>
     <row r="100" spans="1:4" x14ac:dyDescent="0.2">
@@ -2782,10 +2780,10 @@
         <v>1</v>
       </c>
       <c r="C100" t="s">
-        <v>165</v>
+        <v>162</v>
       </c>
       <c r="D100" t="s">
-        <v>170</v>
+        <v>166</v>
       </c>
     </row>
     <row r="101" spans="1:4" x14ac:dyDescent="0.2">
@@ -2796,10 +2794,10 @@
         <v>1</v>
       </c>
       <c r="C101" t="s">
-        <v>165</v>
+        <v>162</v>
       </c>
       <c r="D101" t="s">
-        <v>170</v>
+        <v>166</v>
       </c>
     </row>
     <row r="102" spans="1:4" x14ac:dyDescent="0.2">
@@ -2810,10 +2808,10 @@
         <v>1</v>
       </c>
       <c r="C102" t="s">
-        <v>165</v>
+        <v>162</v>
       </c>
       <c r="D102" t="s">
-        <v>170</v>
+        <v>166</v>
       </c>
     </row>
     <row r="103" spans="1:4" x14ac:dyDescent="0.2">
@@ -2824,10 +2822,10 @@
         <v>1</v>
       </c>
       <c r="C103" t="s">
-        <v>165</v>
+        <v>162</v>
       </c>
       <c r="D103" t="s">
-        <v>170</v>
+        <v>166</v>
       </c>
     </row>
     <row r="104" spans="1:4" x14ac:dyDescent="0.2">
@@ -2838,10 +2836,10 @@
         <v>1</v>
       </c>
       <c r="C104" t="s">
-        <v>165</v>
+        <v>162</v>
       </c>
       <c r="D104" t="s">
-        <v>170</v>
+        <v>166</v>
       </c>
     </row>
     <row r="105" spans="1:4" x14ac:dyDescent="0.2">
@@ -2852,10 +2850,10 @@
         <v>1</v>
       </c>
       <c r="C105" t="s">
-        <v>165</v>
+        <v>162</v>
       </c>
       <c r="D105" t="s">
-        <v>170</v>
+        <v>166</v>
       </c>
     </row>
     <row r="106" spans="1:4" x14ac:dyDescent="0.2">
@@ -2866,10 +2864,10 @@
         <v>1</v>
       </c>
       <c r="C106" t="s">
-        <v>166</v>
+        <v>163</v>
       </c>
       <c r="D106" t="s">
-        <v>169</v>
+        <v>165</v>
       </c>
     </row>
     <row r="107" spans="1:4" x14ac:dyDescent="0.2">
@@ -2880,10 +2878,10 @@
         <v>1</v>
       </c>
       <c r="C107" t="s">
-        <v>165</v>
+        <v>162</v>
       </c>
       <c r="D107" t="s">
-        <v>170</v>
+        <v>166</v>
       </c>
     </row>
     <row r="108" spans="1:4" x14ac:dyDescent="0.2">
@@ -2894,10 +2892,10 @@
         <v>1</v>
       </c>
       <c r="C108" t="s">
-        <v>165</v>
+        <v>162</v>
       </c>
       <c r="D108" t="s">
-        <v>170</v>
+        <v>166</v>
       </c>
     </row>
     <row r="109" spans="1:4" x14ac:dyDescent="0.2">
@@ -2908,10 +2906,10 @@
         <v>1</v>
       </c>
       <c r="C109" t="s">
-        <v>165</v>
+        <v>162</v>
       </c>
       <c r="D109" t="s">
-        <v>170</v>
+        <v>166</v>
       </c>
     </row>
     <row r="110" spans="1:4" x14ac:dyDescent="0.2">
@@ -2922,10 +2920,10 @@
         <v>1</v>
       </c>
       <c r="C110" t="s">
-        <v>165</v>
+        <v>162</v>
       </c>
       <c r="D110" t="s">
-        <v>170</v>
+        <v>166</v>
       </c>
     </row>
     <row r="111" spans="1:4" x14ac:dyDescent="0.2">
@@ -2936,10 +2934,10 @@
         <v>1</v>
       </c>
       <c r="C111" t="s">
-        <v>167</v>
+        <v>164</v>
       </c>
       <c r="D111" t="s">
-        <v>169</v>
+        <v>165</v>
       </c>
     </row>
     <row r="112" spans="1:4" x14ac:dyDescent="0.2">
@@ -2950,10 +2948,10 @@
         <v>1</v>
       </c>
       <c r="C112" t="s">
-        <v>167</v>
+        <v>164</v>
       </c>
       <c r="D112" t="s">
-        <v>169</v>
+        <v>165</v>
       </c>
     </row>
     <row r="113" spans="1:4" x14ac:dyDescent="0.2">
@@ -2964,10 +2962,10 @@
         <v>1</v>
       </c>
       <c r="C113" t="s">
-        <v>167</v>
+        <v>164</v>
       </c>
       <c r="D113" t="s">
-        <v>169</v>
+        <v>165</v>
       </c>
     </row>
     <row r="114" spans="1:4" x14ac:dyDescent="0.2">
@@ -2978,10 +2976,10 @@
         <v>1</v>
       </c>
       <c r="C114" t="s">
-        <v>166</v>
+        <v>163</v>
       </c>
       <c r="D114" t="s">
-        <v>169</v>
+        <v>165</v>
       </c>
     </row>
     <row r="115" spans="1:4" x14ac:dyDescent="0.2">
@@ -2992,10 +2990,10 @@
         <v>1</v>
       </c>
       <c r="C115" t="s">
-        <v>165</v>
+        <v>162</v>
       </c>
       <c r="D115" t="s">
-        <v>170</v>
+        <v>166</v>
       </c>
     </row>
     <row r="116" spans="1:4" x14ac:dyDescent="0.2">
@@ -3006,10 +3004,10 @@
         <v>1</v>
       </c>
       <c r="C116" t="s">
-        <v>165</v>
+        <v>162</v>
       </c>
       <c r="D116" t="s">
-        <v>170</v>
+        <v>166</v>
       </c>
     </row>
     <row r="117" spans="1:4" x14ac:dyDescent="0.2">
@@ -3020,10 +3018,10 @@
         <v>1</v>
       </c>
       <c r="C117" t="s">
-        <v>166</v>
+        <v>163</v>
       </c>
       <c r="D117" t="s">
-        <v>169</v>
+        <v>165</v>
       </c>
     </row>
     <row r="118" spans="1:4" x14ac:dyDescent="0.2">
@@ -3034,10 +3032,10 @@
         <v>1</v>
       </c>
       <c r="C118" t="s">
-        <v>167</v>
+        <v>164</v>
       </c>
       <c r="D118" t="s">
-        <v>169</v>
+        <v>165</v>
       </c>
     </row>
     <row r="119" spans="1:4" x14ac:dyDescent="0.2">
@@ -3048,10 +3046,10 @@
         <v>1</v>
       </c>
       <c r="C119" t="s">
-        <v>167</v>
+        <v>164</v>
       </c>
       <c r="D119" t="s">
-        <v>169</v>
+        <v>165</v>
       </c>
     </row>
     <row r="120" spans="1:4" x14ac:dyDescent="0.2">
@@ -3062,10 +3060,10 @@
         <v>1</v>
       </c>
       <c r="C120" t="s">
-        <v>167</v>
+        <v>164</v>
       </c>
       <c r="D120" t="s">
-        <v>169</v>
+        <v>165</v>
       </c>
     </row>
     <row r="121" spans="1:4" x14ac:dyDescent="0.2">
@@ -3076,10 +3074,10 @@
         <v>1</v>
       </c>
       <c r="C121" t="s">
-        <v>167</v>
+        <v>164</v>
       </c>
       <c r="D121" t="s">
-        <v>169</v>
+        <v>165</v>
       </c>
     </row>
     <row r="122" spans="1:4" x14ac:dyDescent="0.2">
@@ -3090,10 +3088,10 @@
         <v>1</v>
       </c>
       <c r="C122" t="s">
-        <v>167</v>
+        <v>164</v>
       </c>
       <c r="D122" t="s">
-        <v>169</v>
+        <v>165</v>
       </c>
     </row>
     <row r="123" spans="1:4" x14ac:dyDescent="0.2">
@@ -3104,10 +3102,10 @@
         <v>1</v>
       </c>
       <c r="C123" t="s">
-        <v>166</v>
+        <v>163</v>
       </c>
       <c r="D123" t="s">
-        <v>169</v>
+        <v>165</v>
       </c>
     </row>
     <row r="124" spans="1:4" x14ac:dyDescent="0.2">
@@ -3118,10 +3116,10 @@
         <v>1</v>
       </c>
       <c r="C124" t="s">
-        <v>165</v>
+        <v>162</v>
       </c>
       <c r="D124" t="s">
-        <v>170</v>
+        <v>166</v>
       </c>
     </row>
     <row r="125" spans="1:4" x14ac:dyDescent="0.2">
@@ -3132,10 +3130,10 @@
         <v>1</v>
       </c>
       <c r="C125" t="s">
-        <v>165</v>
+        <v>162</v>
       </c>
       <c r="D125" t="s">
-        <v>170</v>
+        <v>166</v>
       </c>
     </row>
     <row r="126" spans="1:4" x14ac:dyDescent="0.2">
@@ -3146,10 +3144,10 @@
         <v>1</v>
       </c>
       <c r="C126" t="s">
-        <v>166</v>
+        <v>163</v>
       </c>
       <c r="D126" t="s">
-        <v>169</v>
+        <v>165</v>
       </c>
     </row>
     <row r="127" spans="1:4" x14ac:dyDescent="0.2">
@@ -3160,10 +3158,10 @@
         <v>1</v>
       </c>
       <c r="C127" t="s">
-        <v>165</v>
+        <v>162</v>
       </c>
       <c r="D127" t="s">
-        <v>170</v>
+        <v>166</v>
       </c>
     </row>
     <row r="128" spans="1:4" x14ac:dyDescent="0.2">
@@ -3174,10 +3172,10 @@
         <v>1</v>
       </c>
       <c r="C128" t="s">
-        <v>165</v>
+        <v>162</v>
       </c>
       <c r="D128" t="s">
-        <v>170</v>
+        <v>166</v>
       </c>
     </row>
     <row r="129" spans="1:4" x14ac:dyDescent="0.2">
@@ -3188,10 +3186,10 @@
         <v>1</v>
       </c>
       <c r="C129" t="s">
-        <v>165</v>
+        <v>162</v>
       </c>
       <c r="D129" t="s">
-        <v>170</v>
+        <v>166</v>
       </c>
     </row>
     <row r="130" spans="1:4" x14ac:dyDescent="0.2">
@@ -3202,10 +3200,10 @@
         <v>1</v>
       </c>
       <c r="C130" t="s">
-        <v>165</v>
+        <v>162</v>
       </c>
       <c r="D130" t="s">
-        <v>170</v>
+        <v>166</v>
       </c>
     </row>
     <row r="131" spans="1:4" x14ac:dyDescent="0.2">
@@ -3216,10 +3214,10 @@
         <v>1</v>
       </c>
       <c r="C131" t="s">
-        <v>165</v>
+        <v>162</v>
       </c>
       <c r="D131" t="s">
-        <v>170</v>
+        <v>166</v>
       </c>
     </row>
     <row r="132" spans="1:4" x14ac:dyDescent="0.2">
@@ -3230,10 +3228,10 @@
         <v>1</v>
       </c>
       <c r="C132" t="s">
-        <v>165</v>
+        <v>162</v>
       </c>
       <c r="D132" t="s">
-        <v>170</v>
+        <v>166</v>
       </c>
     </row>
     <row r="133" spans="1:4" x14ac:dyDescent="0.2">
@@ -3244,10 +3242,10 @@
         <v>1</v>
       </c>
       <c r="C133" t="s">
-        <v>165</v>
+        <v>162</v>
       </c>
       <c r="D133" t="s">
-        <v>170</v>
+        <v>166</v>
       </c>
     </row>
     <row r="134" spans="1:4" x14ac:dyDescent="0.2">
@@ -3258,10 +3256,10 @@
         <v>1</v>
       </c>
       <c r="C134" t="s">
-        <v>165</v>
+        <v>162</v>
       </c>
       <c r="D134" t="s">
-        <v>170</v>
+        <v>166</v>
       </c>
     </row>
     <row r="135" spans="1:4" x14ac:dyDescent="0.2">
@@ -3272,10 +3270,10 @@
         <v>1</v>
       </c>
       <c r="C135" t="s">
-        <v>167</v>
+        <v>164</v>
       </c>
       <c r="D135" t="s">
-        <v>169</v>
+        <v>165</v>
       </c>
     </row>
     <row r="136" spans="1:4" x14ac:dyDescent="0.2">
@@ -3286,10 +3284,10 @@
         <v>1</v>
       </c>
       <c r="C136" t="s">
-        <v>167</v>
+        <v>164</v>
       </c>
       <c r="D136" t="s">
-        <v>169</v>
+        <v>165</v>
       </c>
     </row>
     <row r="137" spans="1:4" x14ac:dyDescent="0.2">
@@ -3300,10 +3298,10 @@
         <v>1</v>
       </c>
       <c r="C137" t="s">
-        <v>167</v>
+        <v>164</v>
       </c>
       <c r="D137" t="s">
-        <v>169</v>
+        <v>165</v>
       </c>
     </row>
     <row r="138" spans="1:4" x14ac:dyDescent="0.2">
@@ -3314,10 +3312,10 @@
         <v>1</v>
       </c>
       <c r="C138" t="s">
-        <v>167</v>
+        <v>164</v>
       </c>
       <c r="D138" t="s">
-        <v>169</v>
+        <v>165</v>
       </c>
     </row>
     <row r="139" spans="1:4" x14ac:dyDescent="0.2">
@@ -3328,10 +3326,10 @@
         <v>1</v>
       </c>
       <c r="C139" t="s">
-        <v>167</v>
+        <v>164</v>
       </c>
       <c r="D139" t="s">
-        <v>169</v>
+        <v>165</v>
       </c>
     </row>
     <row r="140" spans="1:4" x14ac:dyDescent="0.2">
@@ -3342,10 +3340,10 @@
         <v>1</v>
       </c>
       <c r="C140" t="s">
-        <v>165</v>
+        <v>162</v>
       </c>
       <c r="D140" t="s">
-        <v>170</v>
+        <v>166</v>
       </c>
     </row>
     <row r="141" spans="1:4" x14ac:dyDescent="0.2">
@@ -3356,10 +3354,10 @@
         <v>1</v>
       </c>
       <c r="C141" t="s">
-        <v>165</v>
+        <v>162</v>
       </c>
       <c r="D141" t="s">
-        <v>170</v>
+        <v>166</v>
       </c>
     </row>
     <row r="142" spans="1:4" x14ac:dyDescent="0.2">
@@ -3370,10 +3368,10 @@
         <v>1</v>
       </c>
       <c r="C142" t="s">
-        <v>167</v>
+        <v>164</v>
       </c>
       <c r="D142" t="s">
-        <v>169</v>
+        <v>165</v>
       </c>
     </row>
     <row r="143" spans="1:4" x14ac:dyDescent="0.2">
@@ -3384,10 +3382,10 @@
         <v>1</v>
       </c>
       <c r="C143" t="s">
-        <v>167</v>
+        <v>164</v>
       </c>
       <c r="D143" t="s">
-        <v>169</v>
+        <v>165</v>
       </c>
     </row>
     <row r="144" spans="1:4" x14ac:dyDescent="0.2">
@@ -3398,10 +3396,10 @@
         <v>1</v>
       </c>
       <c r="C144" t="s">
-        <v>167</v>
+        <v>164</v>
       </c>
       <c r="D144" t="s">
-        <v>169</v>
+        <v>165</v>
       </c>
     </row>
     <row r="145" spans="1:4" x14ac:dyDescent="0.2">
@@ -3412,10 +3410,10 @@
         <v>1</v>
       </c>
       <c r="C145" t="s">
-        <v>165</v>
+        <v>162</v>
       </c>
       <c r="D145" t="s">
-        <v>170</v>
+        <v>166</v>
       </c>
     </row>
     <row r="146" spans="1:4" x14ac:dyDescent="0.2">
@@ -3426,10 +3424,10 @@
         <v>1</v>
       </c>
       <c r="C146" t="s">
-        <v>166</v>
+        <v>163</v>
       </c>
       <c r="D146" t="s">
-        <v>169</v>
+        <v>165</v>
       </c>
     </row>
     <row r="147" spans="1:4" x14ac:dyDescent="0.2">
@@ -3440,10 +3438,10 @@
         <v>1</v>
       </c>
       <c r="C147" t="s">
-        <v>167</v>
+        <v>164</v>
       </c>
       <c r="D147" t="s">
-        <v>169</v>
+        <v>165</v>
       </c>
     </row>
     <row r="148" spans="1:4" x14ac:dyDescent="0.2">
@@ -3454,10 +3452,10 @@
         <v>1</v>
       </c>
       <c r="C148" t="s">
-        <v>167</v>
+        <v>164</v>
       </c>
       <c r="D148" t="s">
-        <v>169</v>
+        <v>165</v>
       </c>
     </row>
     <row r="149" spans="1:4" x14ac:dyDescent="0.2">
@@ -3468,10 +3466,10 @@
         <v>1</v>
       </c>
       <c r="C149" t="s">
-        <v>167</v>
+        <v>164</v>
       </c>
       <c r="D149" t="s">
-        <v>169</v>
+        <v>165</v>
       </c>
     </row>
     <row r="150" spans="1:4" x14ac:dyDescent="0.2">
@@ -3482,10 +3480,10 @@
         <v>1</v>
       </c>
       <c r="C150" t="s">
-        <v>165</v>
+        <v>162</v>
       </c>
       <c r="D150" t="s">
-        <v>170</v>
+        <v>166</v>
       </c>
     </row>
     <row r="151" spans="1:4" x14ac:dyDescent="0.2">
@@ -3496,10 +3494,10 @@
         <v>1</v>
       </c>
       <c r="C151" t="s">
-        <v>165</v>
+        <v>162</v>
       </c>
       <c r="D151" t="s">
-        <v>170</v>
+        <v>166</v>
       </c>
     </row>
     <row r="152" spans="1:4" x14ac:dyDescent="0.2">
@@ -3510,10 +3508,10 @@
         <v>1</v>
       </c>
       <c r="C152" t="s">
-        <v>166</v>
+        <v>163</v>
       </c>
       <c r="D152" t="s">
-        <v>169</v>
+        <v>165</v>
       </c>
     </row>
     <row r="153" spans="1:4" x14ac:dyDescent="0.2">
@@ -3524,10 +3522,10 @@
         <v>1</v>
       </c>
       <c r="C153" t="s">
-        <v>166</v>
+        <v>163</v>
       </c>
       <c r="D153" t="s">
-        <v>169</v>
+        <v>165</v>
       </c>
     </row>
     <row r="154" spans="1:4" x14ac:dyDescent="0.2">
@@ -3538,10 +3536,10 @@
         <v>1</v>
       </c>
       <c r="C154" t="s">
-        <v>166</v>
+        <v>163</v>
       </c>
       <c r="D154" t="s">
-        <v>169</v>
+        <v>165</v>
       </c>
     </row>
     <row r="155" spans="1:4" x14ac:dyDescent="0.2">
@@ -3552,10 +3550,10 @@
         <v>1</v>
       </c>
       <c r="C155" t="s">
-        <v>166</v>
+        <v>163</v>
       </c>
       <c r="D155" t="s">
-        <v>169</v>
+        <v>165</v>
       </c>
     </row>
     <row r="156" spans="1:4" x14ac:dyDescent="0.2">
@@ -3566,10 +3564,10 @@
         <v>1</v>
       </c>
       <c r="C156" t="s">
-        <v>167</v>
+        <v>164</v>
       </c>
       <c r="D156" t="s">
-        <v>169</v>
+        <v>165</v>
       </c>
     </row>
     <row r="157" spans="1:4" x14ac:dyDescent="0.2">
@@ -3580,10 +3578,10 @@
         <v>1</v>
       </c>
       <c r="C157" t="s">
-        <v>167</v>
+        <v>164</v>
       </c>
       <c r="D157" t="s">
-        <v>169</v>
+        <v>165</v>
       </c>
     </row>
     <row r="158" spans="1:4" x14ac:dyDescent="0.2">
@@ -3594,10 +3592,10 @@
         <v>1</v>
       </c>
       <c r="C158" t="s">
-        <v>167</v>
+        <v>164</v>
       </c>
       <c r="D158" t="s">
-        <v>169</v>
+        <v>165</v>
       </c>
     </row>
     <row r="159" spans="1:4" x14ac:dyDescent="0.2">
@@ -3608,10 +3606,10 @@
         <v>1</v>
       </c>
       <c r="C159" t="s">
-        <v>167</v>
+        <v>164</v>
       </c>
       <c r="D159" t="s">
-        <v>169</v>
+        <v>165</v>
       </c>
     </row>
     <row r="160" spans="1:4" x14ac:dyDescent="0.2">
@@ -3622,10 +3620,10 @@
         <v>1</v>
       </c>
       <c r="C160" t="s">
-        <v>167</v>
+        <v>164</v>
       </c>
       <c r="D160" t="s">
-        <v>169</v>
+        <v>165</v>
       </c>
     </row>
     <row r="161" spans="1:4" x14ac:dyDescent="0.2">
@@ -3636,10 +3634,10 @@
         <v>1</v>
       </c>
       <c r="C161" t="s">
-        <v>167</v>
+        <v>164</v>
       </c>
       <c r="D161" t="s">
-        <v>169</v>
+        <v>165</v>
       </c>
     </row>
     <row r="162" spans="1:4" x14ac:dyDescent="0.2">
@@ -3650,10 +3648,10 @@
         <v>1</v>
       </c>
       <c r="C162" t="s">
-        <v>167</v>
+        <v>164</v>
       </c>
       <c r="D162" t="s">
-        <v>169</v>
+        <v>165</v>
       </c>
     </row>
   </sheetData>

</xml_diff>